<commit_message>
Updating Cronograma del Proyecto
</commit_message>
<xml_diff>
--- a/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
+++ b/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
@@ -1,616 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Desktop\PROYECTOS\FDT-Consulting\02 Desarrollo\SGI\01 Documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisb\Desktop\PROYECTOS\FDT-Consulting\02-Desarrollo\SGI\01-Documentos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9934440B-924A-4A56-8987-2B564EB6C734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45BC3AA6-E7DA-4A2F-A732-1E2F28E39A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cronograma #1" sheetId="1" r:id="rId1"/>
-    <sheet name="IntegrantesRoles" sheetId="2" r:id="rId2"/>
+    <sheet name="Control de Versiones" sheetId="2" r:id="rId2"/>
+    <sheet name="IntegrantesRoles" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="191">
-  <si>
-    <t>CRONOGRAMA DEL PROYECTO</t>
-  </si>
-  <si>
-    <t>Grupo:</t>
-  </si>
-  <si>
-    <t>Proyecto:</t>
-  </si>
-  <si>
-    <t>Sistema de Gestión de Incidencias</t>
-  </si>
-  <si>
-    <t>Enfoque de desarrollo:</t>
-  </si>
-  <si>
-    <t>Scrum</t>
-  </si>
-  <si>
-    <t>Inicio:</t>
-  </si>
-  <si>
-    <t>Fin:</t>
-  </si>
-  <si>
-    <t>Actividad</t>
-  </si>
-  <si>
-    <t>Item</t>
-  </si>
-  <si>
-    <t>Nomenclatura</t>
-  </si>
-  <si>
-    <t>Apellido/Nomenclatura del Rol</t>
-  </si>
-  <si>
-    <t>InicIo</t>
-  </si>
-  <si>
-    <t>Fin</t>
-  </si>
-  <si>
-    <t>% de Avance</t>
-  </si>
-  <si>
-    <t>Reunión con el Stakeholder</t>
-  </si>
-  <si>
-    <t>Acta de Reunión con el stakeholder</t>
-  </si>
-  <si>
-    <t>SGI-AR.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A y Justiniano/A</t>
-  </si>
-  <si>
-    <t>Idear Proyecto innovador</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>S1</t>
-  </si>
-  <si>
-    <t>Desarrollar del Plan de Proyecto</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Plan de Proyecto </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>(PROJECT CHARTER)</t>
-    </r>
-  </si>
-  <si>
-    <t>SGI-PC.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Justiniano/A, Canecillas/A, Del Aguila/QA, Balceda/PB, Soller/PB, Durand/PB, Huarhua/AS</t>
-  </si>
-  <si>
-    <t>S2</t>
-  </si>
-  <si>
-    <t>Elaborar Cronograma del Proyecto</t>
-  </si>
-  <si>
-    <t>Cronograma del Proyecto</t>
-  </si>
-  <si>
-    <t>SGI-CP.XLS</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/DBA-A</t>
-  </si>
-  <si>
-    <t>Crear repositorio del proyecto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Repositorio GitHub
-</t>
-  </si>
-  <si>
-    <t>Balarezo/JP</t>
-  </si>
-  <si>
-    <t>Plan de Elicitación de Requerimientos</t>
-  </si>
-  <si>
-    <t>Documento de Elicitación de Requerimientos</t>
-  </si>
-  <si>
-    <t>SGI-PER.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 1 del Software - Creación de Cuenta</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 1</t>
-  </si>
-  <si>
-    <t>SGI-DER1.DOCX</t>
-  </si>
-  <si>
-    <t>Durand/PB</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 2 del Software - Gestión de Roles</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 2</t>
-  </si>
-  <si>
-    <t>SGI-DER2.DOCX</t>
-  </si>
-  <si>
-    <t>Canecillas/A</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 3 del Software - Autenticación de Usuario</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 3</t>
-  </si>
-  <si>
-    <t>SGI-DER3.DOCX</t>
-  </si>
-  <si>
-    <t>Análisis de Riesgos</t>
-  </si>
-  <si>
-    <t>Documento de Análisis de Riesgos</t>
-  </si>
-  <si>
-    <t>SGI-DAR4.DOCX</t>
-  </si>
-  <si>
-    <t>Del Aguila/QA, Durand/PB</t>
-  </si>
-  <si>
-    <t>Definición de criterios de aceptación</t>
-  </si>
-  <si>
-    <t>Documento de criterios de aceptación</t>
-  </si>
-  <si>
-    <t>SGI-DCA.DOCX</t>
-  </si>
-  <si>
-    <t>Justiniano/A, Canecillas/A, Balceda/PB, Huarhua/AS</t>
-  </si>
-  <si>
-    <t>Validar Historias de Usuario</t>
-  </si>
-  <si>
-    <t>Lista de Historias de Usuario</t>
-  </si>
-  <si>
-    <t>SGI-LHU.DOCX</t>
-  </si>
-  <si>
-    <t>Proponer el diseño inicial de la Interfaz (UI)</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de UI</t>
-  </si>
-  <si>
-    <t>SGI-DEUI1.PDF</t>
-  </si>
-  <si>
-    <t>Huarhua/UX</t>
-  </si>
-  <si>
-    <t>S3 -S4</t>
-  </si>
-  <si>
-    <t>Especificar el diseño de la Base de Datos</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de la BD</t>
-  </si>
-  <si>
-    <t>SGI-DEBD1.DOCX</t>
-  </si>
-  <si>
-    <t>Canecillas/DBA</t>
-  </si>
-  <si>
-    <t>Especificar la Arquitectura y Diseño del Software</t>
-  </si>
-  <si>
-    <t>Documento de Arquitectura del Software</t>
-  </si>
-  <si>
-    <t>SGI-DAS1.DOCX</t>
-  </si>
-  <si>
-    <t>Huarhua/AS</t>
-  </si>
-  <si>
-    <t>S4</t>
-  </si>
-  <si>
-    <t>Realizar análisis de la calidad del software</t>
-  </si>
-  <si>
-    <t>Documento de Análisis de la calidad del software</t>
-  </si>
-  <si>
-    <t>SGI-DACS1.DOCX</t>
-  </si>
-  <si>
-    <t>Del Aguila/QA</t>
-  </si>
-  <si>
-    <t>Reportar estado actual del software</t>
-  </si>
-  <si>
-    <t>Reporte del Desarrollo del Software</t>
-  </si>
-  <si>
-    <t>SGI-RDS1.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB</t>
-  </si>
-  <si>
-    <t>S5</t>
-  </si>
-  <si>
-    <t>Realizar Sprint Retrospective</t>
-  </si>
-  <si>
-    <t>Reporte del Primer Sprint</t>
-  </si>
-  <si>
-    <t>SGI-RPS.DOCX</t>
-  </si>
-  <si>
-    <t>Linea base 1</t>
-  </si>
-  <si>
-    <t>Hito 1 - Fin del Sprint #1</t>
-  </si>
-  <si>
-    <t>Revisión, análisis y validación de los Requisitos y Especificaciones del Software</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requisitos</t>
-  </si>
-  <si>
-    <t>SGI-DERE.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Justiniano/A, Soller/PB</t>
-  </si>
-  <si>
-    <t>S5 - S6</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 4 del Software - Registro de Incidencias</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 4</t>
-  </si>
-  <si>
-    <t>SGI-DER4.DOCX</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 5 del Software - Asignación de Incidencias</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 5</t>
-  </si>
-  <si>
-    <t>SGI-DER5.DOCX</t>
-  </si>
-  <si>
-    <t>Balceda/PB</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 6 del Software - Priorización de Incidencias</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 6</t>
-  </si>
-  <si>
-    <t>SGI-DER6.DOCX</t>
-  </si>
-  <si>
-    <t>Soller/PB</t>
-  </si>
-  <si>
-    <t>Verificar y Actualizar documento de Especificación de UI</t>
-  </si>
-  <si>
-    <t>SGI-DEUI2.PDF</t>
-  </si>
-  <si>
-    <t>Huarhua/UX,  Soller/PB</t>
-  </si>
-  <si>
-    <t>Verificar y Actualizar documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
-    <t>SGI-DEBD2.DOCX</t>
-  </si>
-  <si>
-    <t>Codificación Página Principal</t>
-  </si>
-  <si>
-    <t>Modulo de Página Principal</t>
-  </si>
-  <si>
-    <t>SGI-MPP.DOCX</t>
-  </si>
-  <si>
-    <t>Codificación Autenticación de Usuario (Registro)</t>
-  </si>
-  <si>
-    <t>Módulo de Autenticación de Usuario</t>
-  </si>
-  <si>
-    <t>SGI-MAU.DOCX</t>
-  </si>
-  <si>
-    <t>Justiniano/A, Canecillas/A, Balceda/PB, Huarhua/AS, Durand/PB</t>
-  </si>
-  <si>
-    <t>Codificación Registro de Incidencias</t>
-  </si>
-  <si>
-    <t>Módulo de Registro de Incidencias</t>
-  </si>
-  <si>
-    <t>SGI-MRI.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/A, Justiniano/A, Canecillas/A, Durand/PB</t>
-  </si>
-  <si>
-    <t>Realizar Pruebas de validación del Software</t>
-  </si>
-  <si>
-    <t>Documento de Pruebas de validación del Software</t>
-  </si>
-  <si>
-    <t>SGI-DPVS.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB, Soller/PB</t>
-  </si>
-  <si>
-    <t>Realizar Análisis de la calidad del software</t>
-  </si>
-  <si>
-    <t>SGI-DACS2.DOCX</t>
-  </si>
-  <si>
-    <t>Del Aguila/QA, Soller/PB,  Durand/PB</t>
-  </si>
-  <si>
-    <t>SGI-RDS2.DOCX</t>
-  </si>
-  <si>
-    <t>S7</t>
-  </si>
-  <si>
-    <t>Reporte del Segundo Sprint</t>
-  </si>
-  <si>
-    <t>SGI-RSS.DOCX</t>
-  </si>
-  <si>
-    <t>Linea base 2</t>
-  </si>
-  <si>
-    <t>Hito 2 - Fin del Sprint #2</t>
-  </si>
-  <si>
-    <t>Codificación asignación de personal encargado</t>
-  </si>
-  <si>
-    <t>Módulo de asignación de personal especializado</t>
-  </si>
-  <si>
-    <t>SGI-MAPE.DOCX</t>
-  </si>
-  <si>
-    <t>S7 -S8 - S9</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 7 del Software - Seguimiento de Incidencias</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 7</t>
-  </si>
-  <si>
-    <t>SGI-DER7.DOCX</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 8 del Software - Generación de Reportes</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 8</t>
-  </si>
-  <si>
-    <t>SGI-DER8.DOCX</t>
-  </si>
-  <si>
-    <t>Justiniano/A</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar documento de Especificación de UI</t>
-  </si>
-  <si>
-    <t>SGI-DEUI3.PDF</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
-    <t>SGI-DEBD3.DOCX</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
-  </si>
-  <si>
-    <t>SGI-DAS.DOCX</t>
-  </si>
-  <si>
-    <t>Huarhua/AS, Durand/PB</t>
-  </si>
-  <si>
-    <t>Generar documentación para el usuario</t>
-  </si>
-  <si>
-    <t>Manual de usuario</t>
-  </si>
-  <si>
-    <t>SGI-MU.DOCX</t>
-  </si>
-  <si>
-    <t>Soller/PB, Balceda/PB, Huarhua/UI, Del Aguila/QA</t>
-  </si>
-  <si>
-    <t>Realizar Pruebas de Seguridad del Software</t>
-  </si>
-  <si>
-    <t>Documento de Pruebas del Software</t>
-  </si>
-  <si>
-    <t>SGI-DPS.DOCX</t>
-  </si>
-  <si>
-    <t>Canecillas/A, Del Aguila/QA</t>
-  </si>
-  <si>
-    <t>S9</t>
-  </si>
-  <si>
-    <t>Documento de Análisis de Calidad del Software</t>
-  </si>
-  <si>
-    <t>SGI-DACS3.DOCX</t>
-  </si>
-  <si>
-    <t>SGI-RDS3.DOCX</t>
-  </si>
-  <si>
-    <t>Reporte del Tercer Sprint</t>
-  </si>
-  <si>
-    <t>SGI-RTS.DOCX</t>
-  </si>
-  <si>
-    <t>S9 - S10</t>
-  </si>
-  <si>
-    <t>Elaborar del acta de cierre del proyecto</t>
-  </si>
-  <si>
-    <t>Acta de cierre del proyecto</t>
-  </si>
-  <si>
-    <t>SGI-ACP.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Durand/PB</t>
-  </si>
-  <si>
-    <t>Linea base 3</t>
-  </si>
-  <si>
-    <t>Hito 3 - Fin del Sprint #3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herramienta: </t>
-  </si>
-  <si>
-    <t>GRUPO 5</t>
-  </si>
-  <si>
-    <t>Apellido y nombre</t>
-  </si>
-  <si>
-    <t>Rol</t>
-  </si>
-  <si>
-    <t>Balarezo Ramos, Luis Jesús</t>
-  </si>
-  <si>
-    <t>Jefe de Proyecto / Analista Sr.</t>
-  </si>
-  <si>
-    <t>Durand Caracuzma,Marlon Milko</t>
-  </si>
-  <si>
-    <t>Programador Back-End</t>
-  </si>
-  <si>
-    <t>Del Aguila Febres,Brayan Tadeo</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>Balceda Delgado, Mariana Alejandra</t>
-  </si>
-  <si>
-    <t>Canecillas Contreras,Juan Mariano</t>
-  </si>
-  <si>
-    <t>Analista Senior / DBA</t>
-  </si>
-  <si>
-    <t>Soller Barnechea,Carlos Javier</t>
-  </si>
-  <si>
-    <t>Huarhua Piñas Edson Sebastian</t>
-  </si>
-  <si>
-    <t>Diseñador UI UX / Arquitecto de software</t>
-  </si>
-  <si>
-    <t>Justiniano Quispe,Diego André</t>
-  </si>
-  <si>
-    <t>Analista Sr.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="213">
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
   <si>
     <r>
@@ -635,16 +49,670 @@
       <t>https://github.com/LuisBDev/FDT-Consulting</t>
     </r>
   </si>
+  <si>
+    <t>Grupo:</t>
+  </si>
+  <si>
+    <t>Proyecto:</t>
+  </si>
+  <si>
+    <t>Sistema de Gestión de Incidencias</t>
+  </si>
+  <si>
+    <t>Enfoque de desarrollo:</t>
+  </si>
+  <si>
+    <t>Scrum</t>
+  </si>
+  <si>
+    <t>Inicio:</t>
+  </si>
+  <si>
+    <t>Fin:</t>
+  </si>
+  <si>
+    <t>Actividad</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Nomenclatura</t>
+  </si>
+  <si>
+    <t>Apellido/Nomenclatura del Rol</t>
+  </si>
+  <si>
+    <t>InicIo</t>
+  </si>
+  <si>
+    <t>Fin</t>
+  </si>
+  <si>
+    <t>% de Avance</t>
+  </si>
+  <si>
+    <t>Reunión con el Stakeholder</t>
+  </si>
+  <si>
+    <t>Acta de Reunión con el stakeholder</t>
+  </si>
+  <si>
+    <t>SGI-AR.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A y Justiniano/A</t>
+  </si>
+  <si>
+    <t>Idear Proyecto innovador</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>S1</t>
+  </si>
+  <si>
+    <t>Desarrollar del Plan de Proyecto</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Plan de Proyecto </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>(PROJECT CHARTER)</t>
+    </r>
+  </si>
+  <si>
+    <t>SGI-PC.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Justiniano/A, Canecillas/A, Del Aguila/QA, Balceda/PB, Soller/PB, Durand/PB, Huarhua/AS</t>
+  </si>
+  <si>
+    <t>S2</t>
+  </si>
+  <si>
+    <t>Elaborar Cronograma del Proyecto</t>
+  </si>
+  <si>
+    <t>Cronograma del Proyecto</t>
+  </si>
+  <si>
+    <t>SGI-CP.XLS</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/DBA-A</t>
+  </si>
+  <si>
+    <t>Crear repositorio del proyecto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Repositorio GitHub
+</t>
+  </si>
+  <si>
+    <t>Balarezo/JP</t>
+  </si>
+  <si>
+    <t>Plan de Elicitación de Requerimientos</t>
+  </si>
+  <si>
+    <t>Documento de Elicitación de Requerimientos</t>
+  </si>
+  <si>
+    <t>SGI-PER.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 1 del Software - Creación de Cuenta</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 1</t>
+  </si>
+  <si>
+    <t>SGI-DER1.DOCX</t>
+  </si>
+  <si>
+    <t>Durand/PB</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 2 del Software - Gestión de Roles</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 2</t>
+  </si>
+  <si>
+    <t>SGI-DER2.DOCX</t>
+  </si>
+  <si>
+    <t>Canecillas/A</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 3 del Software - Autenticación de Usuario</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 3</t>
+  </si>
+  <si>
+    <t>SGI-DER3.DOCX</t>
+  </si>
+  <si>
+    <t>Análisis de Riesgos</t>
+  </si>
+  <si>
+    <t>Documento de Análisis de Riesgos</t>
+  </si>
+  <si>
+    <t>SGI-DAR.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Durand/PB</t>
+  </si>
+  <si>
+    <t>Validar Historias de Usuario</t>
+  </si>
+  <si>
+    <t>Lista de Historias de Usuario</t>
+  </si>
+  <si>
+    <t>SGI-LHU.DOCX</t>
+  </si>
+  <si>
+    <t>Justiniano/A, Canecillas/A, Balceda/PB, Huarhua/AS</t>
+  </si>
+  <si>
+    <t>Definición de criterios de aceptación</t>
+  </si>
+  <si>
+    <t>Documento de criterios de aceptación</t>
+  </si>
+  <si>
+    <t>SGI-DCA.DOCX</t>
+  </si>
+  <si>
+    <t>Proponer el diseño inicial de la Interfaz (UI)</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>SGI-DEUI1.DOCX</t>
+  </si>
+  <si>
+    <t>Huarhua/UX</t>
+  </si>
+  <si>
+    <t>S3 -S4</t>
+  </si>
+  <si>
+    <t>Especificar el diseño de la Base de Datos</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de la BD</t>
+  </si>
+  <si>
+    <t>SGI-DEBD1.DOCX</t>
+  </si>
+  <si>
+    <t>Canecillas/DBA</t>
+  </si>
+  <si>
+    <t>Especificar la Arquitectura y Diseño del Software</t>
+  </si>
+  <si>
+    <t>Documento de Arquitectura del Software</t>
+  </si>
+  <si>
+    <t>SGI-DAS1.DOCX</t>
+  </si>
+  <si>
+    <t>Huarhua/AS</t>
+  </si>
+  <si>
+    <t>S4</t>
+  </si>
+  <si>
+    <t>Realizar Sprint Retrospective</t>
+  </si>
+  <si>
+    <t>Reporte del Primer Sprint</t>
+  </si>
+  <si>
+    <t>SGI-RPS.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Soller/PB</t>
+  </si>
+  <si>
+    <t>Documentar Acta de finalización del Hito 1</t>
+  </si>
+  <si>
+    <t>Acta de Finalización Hito 1</t>
+  </si>
+  <si>
+    <t>SGI-AFH1.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Soller/PB, Durand/PB, Balceda/PB</t>
+  </si>
+  <si>
+    <t>Linea base 1</t>
+  </si>
+  <si>
+    <t>Hito 1 - Fin del Sprint #1</t>
+  </si>
+  <si>
+    <t>Revisión, análisis y validación de los Requisitos y Especificaciones del Software</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requisitos</t>
+  </si>
+  <si>
+    <t>SGI-DERE.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A, Justiniano/A, Soller/PB</t>
+  </si>
+  <si>
+    <t>S5 - S6</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 4 del Software - Registro de Incidencias</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 4</t>
+  </si>
+  <si>
+    <t>SGI-DER4.DOCX</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 5 del Software - Asignación de Incidencias</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 5</t>
+  </si>
+  <si>
+    <t>SGI-DER5.DOCX</t>
+  </si>
+  <si>
+    <t>Balceda/PB</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 6 del Software - Priorización de Incidencias</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 6</t>
+  </si>
+  <si>
+    <t>SGI-DER6.DOCX</t>
+  </si>
+  <si>
+    <t>Soller/PB</t>
+  </si>
+  <si>
+    <t>Verificar y Actualizar documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>SGI-DEUI2.PDF</t>
+  </si>
+  <si>
+    <t>Huarhua/UX,  Soller/PB, Del Aguila/QA</t>
+  </si>
+  <si>
+    <t>Verificar y Actualizar documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>SGI-DEBD2.DOCX</t>
+  </si>
+  <si>
+    <t>Canecillas/DBA, Soller/PB</t>
+  </si>
+  <si>
+    <t>Codificación Página Principal</t>
+  </si>
+  <si>
+    <t>Modulo de Página Principal</t>
+  </si>
+  <si>
+    <t>SGI-MPP.DOCX</t>
+  </si>
+  <si>
+    <t>Soller/PB, Canecillas/A, Balceda/PB, Huarhua/AS</t>
+  </si>
+  <si>
+    <t>Codificación Autenticación de Usuario (Registro)</t>
+  </si>
+  <si>
+    <t>Módulo de Autenticación de Usuario</t>
+  </si>
+  <si>
+    <t>SGI-MAU.DOCX</t>
+  </si>
+  <si>
+    <t>Justiniano/A, Canecillas/A, Balceda/PB, Huarhua/AS, Durand/PB</t>
+  </si>
+  <si>
+    <t>Codificación Registro de Incidencias</t>
+  </si>
+  <si>
+    <t>Módulo de Registro de Incidencias</t>
+  </si>
+  <si>
+    <t>SGI-MRI.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/A, Justiniano/A, Canecillas/A, Durand/PB</t>
+  </si>
+  <si>
+    <t>Realizar Pruebas de validación del Software</t>
+  </si>
+  <si>
+    <t>Documento de Pruebas de validación del Software</t>
+  </si>
+  <si>
+    <t>SGI-DPVS.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB, Soller/PB</t>
+  </si>
+  <si>
+    <t>Realizar Análisis de la calidad del software</t>
+  </si>
+  <si>
+    <t>Documento de Análisis de la calidad del software</t>
+  </si>
+  <si>
+    <t>SGI-DACS2.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Soller/PB,  Durand/PB</t>
+  </si>
+  <si>
+    <t>Reportar estado actual del software</t>
+  </si>
+  <si>
+    <t>Reporte del Desarrollo del Software</t>
+  </si>
+  <si>
+    <t>SGI-RDS2.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>Reporte del Segundo Sprint</t>
+  </si>
+  <si>
+    <t>SGI-RSS.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A, Balceda/PB</t>
+  </si>
+  <si>
+    <t>Documentar Acta de finalización del Hito 2</t>
+  </si>
+  <si>
+    <t>Acta de Finalización Hito 2</t>
+  </si>
+  <si>
+    <t>SGI-AFH2.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Del Aguila/QA, Soller/PB</t>
+  </si>
+  <si>
+    <t>Linea base 2</t>
+  </si>
+  <si>
+    <t>Hito 2 - Fin del Sprint #2</t>
+  </si>
+  <si>
+    <t>Codificación asignación de personal encargado</t>
+  </si>
+  <si>
+    <t>Módulo de asignación de personal especializado</t>
+  </si>
+  <si>
+    <t>SGI-MAPE.DOCX</t>
+  </si>
+  <si>
+    <t>S7 -S8 - S9</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 7 del Software - Seguimiento de Incidencias</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 7</t>
+  </si>
+  <si>
+    <t>SGI-DER7.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 8 del Software - Generación de Reportes</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 8</t>
+  </si>
+  <si>
+    <t>SGI-DER8.DOCX</t>
+  </si>
+  <si>
+    <t>Justiniano/A</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>SGI-DEUI3.PDF</t>
+  </si>
+  <si>
+    <t>Huarhua/UX,  Soller/PB</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>SGI-DEBD3.DOCX</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
+  </si>
+  <si>
+    <t>SGI-DAS.DOCX</t>
+  </si>
+  <si>
+    <t>Huarhua/AS, Durand/PB</t>
+  </si>
+  <si>
+    <t>Generar documentación para el usuario</t>
+  </si>
+  <si>
+    <t>Manual de usuario</t>
+  </si>
+  <si>
+    <t>SGI-MU.DOCX</t>
+  </si>
+  <si>
+    <t>Soller/PB, Balceda/PB, Huarhua/UI, Del Aguila/QA</t>
+  </si>
+  <si>
+    <t>Realizar Pruebas de Seguridad del Software</t>
+  </si>
+  <si>
+    <t>Documento de Pruebas del Software</t>
+  </si>
+  <si>
+    <t>SGI-DPS.DOCX</t>
+  </si>
+  <si>
+    <t>Canecillas/A, Del Aguila/QA</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>Documento de Análisis de Calidad del Software</t>
+  </si>
+  <si>
+    <t>SGI-DACS3.DOCX</t>
+  </si>
+  <si>
+    <t>SGI-RDS3.DOCX</t>
+  </si>
+  <si>
+    <t>Reporte del Tercer Sprint</t>
+  </si>
+  <si>
+    <t>SGI-RTS.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Justiniano/A, Huarhua/AS</t>
+  </si>
+  <si>
+    <t>S9 - S10</t>
+  </si>
+  <si>
+    <t>Documentar Acta de finalización del Hito 3</t>
+  </si>
+  <si>
+    <t>Acta de Finalización Hito 3</t>
+  </si>
+  <si>
+    <t>SGI-AFH3.DOCX</t>
+  </si>
+  <si>
+    <t>Elaborar del acta de cierre del proyecto</t>
+  </si>
+  <si>
+    <t>Acta de cierre del proyecto</t>
+  </si>
+  <si>
+    <t>SGI-ACP.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Canecillas/A, Durand/PB</t>
+  </si>
+  <si>
+    <t>Linea base 3</t>
+  </si>
+  <si>
+    <t>Hito 3 - Fin del Sprint #3</t>
+  </si>
+  <si>
+    <t>Versión</t>
+  </si>
+  <si>
+    <t>Fecha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autor </t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Luis Balarezo</t>
+  </si>
+  <si>
+    <t>Creación del Cronograma del Proyecto</t>
+  </si>
+  <si>
+    <t>Reorganización de 2 artefactos del hito 1 debido a que no correspondían a dicho hito</t>
+  </si>
+  <si>
+    <t>Se agregó ítem de acta de finalización para el Hito 1, 2 y 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Herramienta: </t>
+  </si>
+  <si>
+    <t>GRUPO 5</t>
+  </si>
+  <si>
+    <t>Apellido y nombre</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Balarezo Ramos, Luis Jesús</t>
+  </si>
+  <si>
+    <t>Jefe de Proyecto / Analista Sr.</t>
+  </si>
+  <si>
+    <t>Durand Caracuzma,Marlon Milko</t>
+  </si>
+  <si>
+    <t>Programador Back-End</t>
+  </si>
+  <si>
+    <t>Del Aguila Febres,Brayan Tadeo</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Balceda Delgado, Mariana Alejandra</t>
+  </si>
+  <si>
+    <t>Canecillas Contreras,Juan Mariano</t>
+  </si>
+  <si>
+    <t>Analista Senior / DBA</t>
+  </si>
+  <si>
+    <t>Soller Barnechea,Carlos Javier</t>
+  </si>
+  <si>
+    <t>Huarhua Piñas Edson Sebastian</t>
+  </si>
+  <si>
+    <t>Diseñador UI UX / Arquitecto de software</t>
+  </si>
+  <si>
+    <t>Justiniano Quispe,Diego André</t>
+  </si>
+  <si>
+    <t>Analista Sr.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
+    <numFmt numFmtId="166" formatCode="d\.m"/>
   </numFmts>
-  <fonts count="31">
+  <fonts count="33">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -806,6 +874,17 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Montserrat"/>
@@ -831,7 +910,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -892,8 +971,14 @@
         <bgColor rgb="FFDEFFED"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF9FC5E8"/>
+        <bgColor rgb="FF9FC5E8"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="26">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -1213,6 +1298,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thick">
         <color rgb="FF000000"/>
       </left>
@@ -1242,7 +1351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1372,26 +1481,47 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="29" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1403,7 +1533,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="28" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1624,42 +1754,42 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:K1010"/>
+  <dimension ref="A1:K1011"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
-    <col min="2" max="2" width="69.42578125" customWidth="1"/>
-    <col min="3" max="3" width="53" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="69.28515625" customWidth="1"/>
-    <col min="6" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="10.140625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" customWidth="1"/>
+    <col min="2" max="2" width="69.44140625" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.21875" customWidth="1"/>
+    <col min="5" max="5" width="46.109375" customWidth="1"/>
+    <col min="6" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="14.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="32.25" customHeight="1">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="72"/>
-      <c r="C1" s="72"/>
-      <c r="D1" s="72"/>
-      <c r="E1" s="72"/>
-      <c r="F1" s="72"/>
-      <c r="G1" s="72"/>
-      <c r="H1" s="72"/>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
     </row>
     <row r="2" spans="1:11" ht="15.75" customHeight="1">
       <c r="A2" s="1"/>
-      <c r="B2" s="74" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="75"/>
+      <c r="B2" s="81" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="82"/>
       <c r="D2" s="2"/>
       <c r="E2" s="1"/>
       <c r="F2" s="3"/>
@@ -1669,7 +1799,7 @@
     <row r="3" spans="1:11" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="5" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3" s="6">
         <v>5</v>
@@ -1683,10 +1813,10 @@
     <row r="4" spans="1:11" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="5" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
@@ -1697,10 +1827,10 @@
     <row r="5" spans="1:11" ht="15.75" customHeight="1">
       <c r="A5" s="1"/>
       <c r="B5" s="5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
@@ -1711,7 +1841,7 @@
     <row r="6" spans="1:11" ht="15.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C6" s="8">
         <v>45026</v>
@@ -1725,7 +1855,7 @@
     <row r="7" spans="1:11" ht="15.75" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C7" s="10">
         <v>45107</v>
@@ -1745,40 +1875,40 @@
     <row r="9" spans="1:11" ht="15.75" customHeight="1">
       <c r="A9" s="11"/>
       <c r="B9" s="13" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D9" s="14" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H9" s="16" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1">
       <c r="A10" s="11"/>
       <c r="B10" s="17" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" s="21">
         <v>45019</v>
@@ -1795,13 +1925,13 @@
     <row r="11" spans="1:11" ht="15.75" customHeight="1">
       <c r="A11" s="11"/>
       <c r="B11" s="17" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E11" s="20"/>
       <c r="F11" s="21">
@@ -1814,23 +1944,23 @@
         <v>1</v>
       </c>
       <c r="I11" s="23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="J11" s="2"/>
     </row>
-    <row r="12" spans="1:11" ht="24.75" customHeight="1">
+    <row r="12" spans="1:11" ht="31.5" customHeight="1">
       <c r="A12" s="11"/>
       <c r="B12" s="17" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E12" s="20" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F12" s="21">
         <v>45020</v>
@@ -1841,8 +1971,8 @@
       <c r="H12" s="22">
         <v>1</v>
       </c>
-      <c r="I12" s="71" t="s">
-        <v>26</v>
+      <c r="I12" s="78" t="s">
+        <v>27</v>
       </c>
       <c r="J12" s="26"/>
       <c r="K12" s="2"/>
@@ -1850,16 +1980,16 @@
     <row r="13" spans="1:11" ht="15.75" customHeight="1">
       <c r="A13" s="11"/>
       <c r="B13" s="17" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C13" s="27" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="20" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F13" s="21">
         <v>45022</v>
@@ -1870,22 +2000,22 @@
       <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="I13" s="72"/>
+      <c r="I13" s="79"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1">
       <c r="A14" s="11"/>
       <c r="B14" s="17" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C14" s="28" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E14" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F14" s="21">
         <v>45024</v>
@@ -1896,22 +2026,22 @@
       <c r="H14" s="22">
         <v>1</v>
       </c>
-      <c r="I14" s="72"/>
+      <c r="I14" s="79"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:11" ht="16.5" customHeight="1">
       <c r="A15" s="11"/>
       <c r="B15" s="17" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15" s="28" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="D15" s="24" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E15" s="20" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="F15" s="21">
         <v>45024</v>
@@ -1922,23 +2052,23 @@
       <c r="H15" s="22">
         <v>1</v>
       </c>
-      <c r="I15" s="72"/>
+      <c r="I15" s="79"/>
       <c r="J15" s="26"/>
       <c r="K15" s="2"/>
     </row>
     <row r="16" spans="1:11" ht="16.5" customHeight="1">
       <c r="A16" s="11"/>
       <c r="B16" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="E16" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F16" s="21">
         <v>45024</v>
@@ -1947,25 +2077,25 @@
         <v>45038</v>
       </c>
       <c r="H16" s="22">
-        <v>0</v>
-      </c>
-      <c r="I16" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="79"/>
       <c r="J16" s="26"/>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" ht="16.5" customHeight="1">
       <c r="A17" s="11"/>
       <c r="B17" s="29" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F17" s="21">
         <v>45024</v>
@@ -1974,25 +2104,25 @@
         <v>45038</v>
       </c>
       <c r="H17" s="22">
-        <v>0</v>
-      </c>
-      <c r="I17" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="79"/>
       <c r="J17" s="26"/>
       <c r="K17" s="2"/>
     </row>
     <row r="18" spans="1:11" ht="16.5" customHeight="1">
       <c r="A18" s="11"/>
       <c r="B18" s="17" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C18" s="28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D18" s="24" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F18" s="21">
         <v>45024</v>
@@ -2001,25 +2131,25 @@
         <v>45038</v>
       </c>
       <c r="H18" s="22">
-        <v>0</v>
-      </c>
-      <c r="I18" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I18" s="79"/>
       <c r="J18" s="26"/>
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="16.5" customHeight="1">
       <c r="A19" s="11"/>
       <c r="B19" s="17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C19" s="28" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D19" s="24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="E19" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F19" s="21">
         <v>45024</v>
@@ -2028,25 +2158,25 @@
         <v>45040</v>
       </c>
       <c r="H19" s="22">
-        <v>0</v>
-      </c>
-      <c r="I19" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="79"/>
       <c r="J19" s="26"/>
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11" ht="16.5" customHeight="1">
       <c r="A20" s="11"/>
       <c r="B20" s="17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C20" s="28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D20" s="24" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E20" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F20" s="21">
         <v>45040</v>
@@ -2055,25 +2185,25 @@
         <v>45042</v>
       </c>
       <c r="H20" s="22">
-        <v>0</v>
-      </c>
-      <c r="I20" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I20" s="79"/>
       <c r="J20" s="26"/>
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11" ht="18" customHeight="1">
       <c r="A21" s="11"/>
       <c r="B21" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="E21" s="20" t="s">
         <v>57</v>
-      </c>
-      <c r="C21" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D21" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>56</v>
       </c>
       <c r="F21" s="21">
         <v>45040</v>
@@ -2082,25 +2212,25 @@
         <v>45042</v>
       </c>
       <c r="H21" s="22">
-        <v>0</v>
-      </c>
-      <c r="I21" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I21" s="79"/>
       <c r="J21" s="26"/>
       <c r="K21" s="2"/>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1">
       <c r="A22" s="11"/>
       <c r="B22" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C22" s="28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D22" s="24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E22" s="20" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="F22" s="21">
         <v>45041</v>
@@ -2109,10 +2239,10 @@
         <v>45045</v>
       </c>
       <c r="H22" s="22">
-        <v>0</v>
-      </c>
-      <c r="I22" s="71" t="s">
-        <v>64</v>
+        <v>1</v>
+      </c>
+      <c r="I22" s="78" t="s">
+        <v>65</v>
       </c>
       <c r="J22" s="26"/>
       <c r="K22" s="2"/>
@@ -2120,16 +2250,16 @@
     <row r="23" spans="1:11" ht="15.75" customHeight="1">
       <c r="A23" s="11"/>
       <c r="B23" s="33" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D23" s="24" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F23" s="21">
         <v>45041</v>
@@ -2138,25 +2268,25 @@
         <v>45045</v>
       </c>
       <c r="H23" s="22">
-        <v>0</v>
-      </c>
-      <c r="I23" s="72"/>
+        <v>1</v>
+      </c>
+      <c r="I23" s="79"/>
       <c r="J23" s="26"/>
       <c r="K23" s="2"/>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1">
       <c r="A24" s="11"/>
       <c r="B24" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C24" s="28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D24" s="24" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F24" s="21">
         <v>45043</v>
@@ -2165,10 +2295,10 @@
         <v>45045</v>
       </c>
       <c r="H24" s="22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I24" s="23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="J24" s="26"/>
       <c r="K24" s="2"/>
@@ -2176,147 +2306,145 @@
     <row r="25" spans="1:11" ht="15.75" customHeight="1">
       <c r="A25" s="11"/>
       <c r="B25" s="17" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C25" s="28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D25" s="24" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F25" s="21">
         <v>45045</v>
       </c>
       <c r="G25" s="21">
-        <v>45047</v>
+        <v>45049</v>
       </c>
       <c r="H25" s="22">
-        <v>0</v>
-      </c>
-      <c r="I25" s="23"/>
+        <v>1</v>
+      </c>
+      <c r="I25" s="78"/>
       <c r="J25" s="26"/>
       <c r="K25" s="2"/>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1">
       <c r="A26" s="11"/>
       <c r="B26" s="17" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C26" s="28" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D26" s="24" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F26" s="21">
-        <v>45047</v>
+        <v>45049</v>
       </c>
       <c r="G26" s="21">
-        <v>45048</v>
+        <v>45050</v>
       </c>
       <c r="H26" s="22">
-        <v>0</v>
-      </c>
-      <c r="I26" s="71" t="s">
-        <v>82</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="I26" s="79"/>
       <c r="J26" s="26"/>
       <c r="K26" s="2"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="17" t="s">
+      <c r="A27" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="B27" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="D27" s="24" t="s">
+      <c r="C27" s="36"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="37"/>
+      <c r="F27" s="38">
+        <v>45019</v>
+      </c>
+      <c r="G27" s="38">
+        <v>45050</v>
+      </c>
+      <c r="H27" s="39"/>
+      <c r="I27" s="79"/>
+    </row>
+    <row r="28" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A28" s="11"/>
+      <c r="B28" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E27" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F27" s="21">
-        <v>45048</v>
-      </c>
-      <c r="G27" s="21">
-        <v>45050</v>
-      </c>
-      <c r="H27" s="22">
+      <c r="C28" s="28" t="s">
+        <v>86</v>
+      </c>
+      <c r="D28" s="24" t="s">
+        <v>87</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="21">
+        <v>45051</v>
+      </c>
+      <c r="G28" s="21">
+        <v>45053</v>
+      </c>
+      <c r="H28" s="41">
         <v>0</v>
       </c>
-      <c r="I27" s="72"/>
-      <c r="J27" s="26"/>
-      <c r="K27" s="2"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A28" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" s="36"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="38">
-        <v>45019</v>
-      </c>
-      <c r="G28" s="38">
-        <v>45050</v>
-      </c>
-      <c r="H28" s="39"/>
-      <c r="I28" s="72"/>
+      <c r="I28" s="78" t="s">
+        <v>89</v>
+      </c>
+      <c r="J28" s="26"/>
+      <c r="K28" s="2"/>
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1">
       <c r="A29" s="11"/>
-      <c r="B29" s="40" t="s">
-        <v>88</v>
+      <c r="B29" s="17" t="s">
+        <v>90</v>
       </c>
       <c r="C29" s="28" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="D29" s="24" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E29" s="20" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="F29" s="21">
-        <v>45051</v>
+        <v>45053</v>
       </c>
       <c r="G29" s="21">
-        <v>45053</v>
-      </c>
-      <c r="H29" s="41">
+        <v>45063</v>
+      </c>
+      <c r="H29" s="22">
         <v>0</v>
       </c>
-      <c r="I29" s="71" t="s">
-        <v>92</v>
-      </c>
+      <c r="I29" s="79"/>
       <c r="J29" s="26"/>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1">
       <c r="A30" s="11"/>
-      <c r="B30" s="17" t="s">
+      <c r="B30" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="E30" s="20" t="s">
-        <v>72</v>
+      <c r="E30" s="32" t="s">
+        <v>96</v>
       </c>
       <c r="F30" s="21">
         <v>45053</v>
@@ -2327,23 +2455,23 @@
       <c r="H30" s="22">
         <v>0</v>
       </c>
-      <c r="I30" s="72"/>
+      <c r="I30" s="79"/>
       <c r="J30" s="26"/>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1">
       <c r="A31" s="11"/>
-      <c r="B31" s="29" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31" s="30" t="s">
+      <c r="B31" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="C31" s="28" t="s">
         <v>98</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="D31" s="24" t="s">
         <v>99</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>100</v>
       </c>
       <c r="F31" s="21">
         <v>45053</v>
@@ -2354,17 +2482,17 @@
       <c r="H31" s="22">
         <v>0</v>
       </c>
-      <c r="I31" s="72"/>
+      <c r="I31" s="79"/>
       <c r="J31" s="26"/>
       <c r="K31" s="2"/>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1">
       <c r="A32" s="11"/>
-      <c r="B32" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="C32" s="28" t="s">
+      <c r="B32" s="40" t="s">
         <v>101</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>62</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>102</v>
@@ -2373,25 +2501,25 @@
         <v>103</v>
       </c>
       <c r="F32" s="21">
-        <v>45053</v>
+        <v>45056</v>
       </c>
       <c r="G32" s="21">
-        <v>45063</v>
-      </c>
-      <c r="H32" s="22">
+        <v>45066</v>
+      </c>
+      <c r="H32" s="42">
         <v>0</v>
       </c>
-      <c r="I32" s="72"/>
+      <c r="I32" s="79"/>
       <c r="J32" s="26"/>
       <c r="K32" s="2"/>
     </row>
     <row r="33" spans="1:11" ht="15.75" customHeight="1">
       <c r="A33" s="11"/>
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="43" t="s">
         <v>104</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D33" s="24" t="s">
         <v>105</v>
@@ -2400,58 +2528,58 @@
         <v>106</v>
       </c>
       <c r="F33" s="21">
-        <v>45056</v>
+        <v>45058</v>
       </c>
       <c r="G33" s="21">
         <v>45066</v>
       </c>
-      <c r="H33" s="42">
+      <c r="H33" s="41">
         <v>0</v>
       </c>
-      <c r="I33" s="72"/>
+      <c r="I33" s="79"/>
       <c r="J33" s="26"/>
       <c r="K33" s="2"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1">
+    <row r="34" spans="1:11" ht="22.5" customHeight="1">
       <c r="A34" s="11"/>
-      <c r="B34" s="43" t="s">
+      <c r="B34" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C34" s="34" t="s">
-        <v>66</v>
+      <c r="C34" s="28" t="s">
+        <v>108</v>
       </c>
       <c r="D34" s="24" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>68</v>
+        <v>110</v>
       </c>
       <c r="F34" s="21">
         <v>45058</v>
       </c>
       <c r="G34" s="21">
-        <v>45066</v>
-      </c>
-      <c r="H34" s="41">
+        <v>45070</v>
+      </c>
+      <c r="H34" s="42">
         <v>0</v>
       </c>
-      <c r="I34" s="72"/>
+      <c r="I34" s="79"/>
       <c r="J34" s="26"/>
       <c r="K34" s="2"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+    <row r="35" spans="1:11" ht="26.25" customHeight="1">
       <c r="A35" s="11"/>
       <c r="B35" s="17" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C35" s="28" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D35" s="24" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>56</v>
+        <v>114</v>
       </c>
       <c r="F35" s="21">
         <v>45058</v>
@@ -2462,23 +2590,23 @@
       <c r="H35" s="42">
         <v>0</v>
       </c>
-      <c r="I35" s="72"/>
+      <c r="I35" s="79"/>
       <c r="J35" s="26"/>
       <c r="K35" s="2"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+    <row r="36" spans="1:11" ht="24" customHeight="1">
       <c r="A36" s="11"/>
       <c r="B36" s="17" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="C36" s="28" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="D36" s="24" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="E36" s="20" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="F36" s="21">
         <v>45058</v>
@@ -2489,29 +2617,29 @@
       <c r="H36" s="42">
         <v>0</v>
       </c>
-      <c r="I36" s="72"/>
+      <c r="I36" s="23"/>
       <c r="J36" s="26"/>
       <c r="K36" s="2"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1">
+    <row r="37" spans="1:11" ht="24.75" customHeight="1">
       <c r="A37" s="11"/>
       <c r="B37" s="17" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="C37" s="28" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="E37" s="20" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F37" s="21">
-        <v>45058</v>
+        <v>45070</v>
       </c>
       <c r="G37" s="21">
-        <v>45070</v>
+        <v>45077</v>
       </c>
       <c r="H37" s="42">
         <v>0</v>
@@ -2523,19 +2651,19 @@
     <row r="38" spans="1:11" ht="15.75" customHeight="1">
       <c r="A38" s="11"/>
       <c r="B38" s="17" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="C38" s="28" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="E38" s="20" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F38" s="21">
-        <v>45070</v>
+        <v>45072</v>
       </c>
       <c r="G38" s="21">
         <v>45077</v>
@@ -2550,16 +2678,16 @@
     <row r="39" spans="1:11" ht="15.75" customHeight="1">
       <c r="A39" s="11"/>
       <c r="B39" s="17" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="C39" s="28" t="s">
-        <v>75</v>
+        <v>128</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>125</v>
+        <v>129</v>
       </c>
       <c r="E39" s="20" t="s">
-        <v>126</v>
+        <v>130</v>
       </c>
       <c r="F39" s="21">
         <v>45072</v>
@@ -2567,29 +2695,31 @@
       <c r="G39" s="21">
         <v>45077</v>
       </c>
-      <c r="H39" s="42">
+      <c r="H39" s="22">
         <v>0</v>
       </c>
-      <c r="I39" s="23"/>
+      <c r="I39" s="78" t="s">
+        <v>131</v>
+      </c>
       <c r="J39" s="26"/>
       <c r="K39" s="2"/>
     </row>
     <row r="40" spans="1:11" ht="15.75" customHeight="1">
       <c r="A40" s="11"/>
       <c r="B40" s="17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C40" s="28" t="s">
-        <v>79</v>
+        <v>132</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c r="E40" s="20" t="s">
-        <v>81</v>
+        <v>134</v>
       </c>
       <c r="F40" s="21">
-        <v>45072</v>
+        <v>45074</v>
       </c>
       <c r="G40" s="21">
         <v>45077</v>
@@ -2597,25 +2727,23 @@
       <c r="H40" s="22">
         <v>0</v>
       </c>
-      <c r="I40" s="71" t="s">
-        <v>128</v>
-      </c>
+      <c r="I40" s="79"/>
       <c r="J40" s="26"/>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:11" ht="15.75" customHeight="1">
       <c r="A41" s="11"/>
       <c r="B41" s="17" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="C41" s="28" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>37</v>
+        <v>138</v>
       </c>
       <c r="F41" s="21">
         <v>45074</v>
@@ -2626,16 +2754,16 @@
       <c r="H41" s="22">
         <v>0</v>
       </c>
-      <c r="I41" s="72"/>
+      <c r="I41" s="79"/>
       <c r="J41" s="26"/>
       <c r="K41" s="2"/>
     </row>
     <row r="42" spans="1:11" ht="15.75" customHeight="1">
       <c r="A42" s="11" t="s">
-        <v>131</v>
+        <v>139</v>
       </c>
       <c r="B42" s="35" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C42" s="44"/>
       <c r="D42" s="45"/>
@@ -2647,21 +2775,21 @@
         <v>45077</v>
       </c>
       <c r="H42" s="46"/>
-      <c r="I42" s="72"/>
+      <c r="I42" s="79"/>
     </row>
     <row r="43" spans="1:11" ht="15.75" customHeight="1">
       <c r="A43" s="11"/>
       <c r="B43" s="47" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C43" s="28" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="E43" s="20" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F43" s="21">
         <v>45078</v>
@@ -2672,8 +2800,8 @@
       <c r="H43" s="22">
         <v>0</v>
       </c>
-      <c r="I43" s="71" t="s">
-        <v>136</v>
+      <c r="I43" s="78" t="s">
+        <v>144</v>
       </c>
       <c r="J43" s="26"/>
       <c r="K43" s="2"/>
@@ -2681,16 +2809,16 @@
     <row r="44" spans="1:11" ht="15.75" customHeight="1">
       <c r="A44" s="11"/>
       <c r="B44" s="17" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="C44" s="28" t="s">
-        <v>138</v>
+        <v>146</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="E44" s="20" t="s">
-        <v>77</v>
+        <v>148</v>
       </c>
       <c r="F44" s="21">
         <v>45078</v>
@@ -2701,23 +2829,23 @@
       <c r="H44" s="22">
         <v>0</v>
       </c>
-      <c r="I44" s="72"/>
+      <c r="I44" s="79"/>
       <c r="J44" s="26"/>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:11" ht="15.75" customHeight="1">
       <c r="A45" s="11"/>
       <c r="B45" s="29" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C45" s="30" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D45" s="31" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="F45" s="21">
         <v>45078</v>
@@ -2728,23 +2856,23 @@
       <c r="H45" s="22">
         <v>0</v>
       </c>
-      <c r="I45" s="72"/>
+      <c r="I45" s="79"/>
       <c r="J45" s="26"/>
       <c r="K45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="15.75" customHeight="1">
       <c r="A46" s="11"/>
       <c r="B46" s="48" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="C46" s="34" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="E46" s="20" t="s">
-        <v>106</v>
+        <v>155</v>
       </c>
       <c r="F46" s="21">
         <v>45080</v>
@@ -2755,23 +2883,23 @@
       <c r="H46" s="22">
         <v>0</v>
       </c>
-      <c r="I46" s="72"/>
+      <c r="I46" s="79"/>
       <c r="J46" s="26"/>
       <c r="K46" s="2"/>
     </row>
     <row r="47" spans="1:11" ht="15.75" customHeight="1">
       <c r="A47" s="11"/>
       <c r="B47" s="49" t="s">
-        <v>146</v>
+        <v>156</v>
       </c>
       <c r="C47" s="34" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>147</v>
+        <v>157</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F47" s="21">
         <v>45080</v>
@@ -2782,23 +2910,23 @@
       <c r="H47" s="22">
         <v>0</v>
       </c>
-      <c r="I47" s="72"/>
+      <c r="I47" s="79"/>
       <c r="J47" s="26"/>
       <c r="K47" s="2"/>
     </row>
     <row r="48" spans="1:11" ht="15.75" customHeight="1">
       <c r="A48" s="11"/>
       <c r="B48" s="47" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="C48" s="28" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="E48" s="20" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="F48" s="21">
         <v>45081</v>
@@ -2809,23 +2937,23 @@
       <c r="H48" s="22">
         <v>0</v>
       </c>
-      <c r="I48" s="72"/>
+      <c r="I48" s="79"/>
       <c r="J48" s="26"/>
       <c r="K48" s="2"/>
     </row>
     <row r="49" spans="1:11" ht="14.25" customHeight="1">
       <c r="A49" s="11"/>
       <c r="B49" s="47" t="s">
-        <v>151</v>
+        <v>161</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>152</v>
+        <v>162</v>
       </c>
       <c r="D49" s="24" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="E49" s="20" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
       <c r="F49" s="21">
         <v>45086</v>
@@ -2836,23 +2964,23 @@
       <c r="H49" s="22">
         <v>0</v>
       </c>
-      <c r="I49" s="72"/>
+      <c r="I49" s="79"/>
       <c r="J49" s="26"/>
       <c r="K49" s="2"/>
     </row>
     <row r="50" spans="1:11" ht="15.75" customHeight="1">
       <c r="A50" s="11"/>
       <c r="B50" s="47" t="s">
-        <v>155</v>
+        <v>165</v>
       </c>
       <c r="C50" s="28" t="s">
-        <v>156</v>
+        <v>166</v>
       </c>
       <c r="D50" s="24" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
       <c r="E50" s="20" t="s">
-        <v>158</v>
+        <v>168</v>
       </c>
       <c r="F50" s="21">
         <v>45097</v>
@@ -2863,8 +2991,8 @@
       <c r="H50" s="22">
         <v>0</v>
       </c>
-      <c r="I50" s="71" t="s">
-        <v>159</v>
+      <c r="I50" s="78" t="s">
+        <v>169</v>
       </c>
       <c r="J50" s="26"/>
       <c r="K50" s="2"/>
@@ -2872,16 +3000,16 @@
     <row r="51" spans="1:11" ht="15.75" customHeight="1">
       <c r="A51" s="11"/>
       <c r="B51" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="D51" s="24" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="E51" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="F51" s="21">
         <v>45101</v>
@@ -2892,23 +3020,23 @@
       <c r="H51" s="22">
         <v>0</v>
       </c>
-      <c r="I51" s="72"/>
+      <c r="I51" s="79"/>
       <c r="J51" s="26"/>
       <c r="K51" s="2"/>
     </row>
     <row r="52" spans="1:11" ht="15.75" customHeight="1">
       <c r="A52" s="11"/>
       <c r="B52" s="47" t="s">
-        <v>78</v>
+        <v>127</v>
       </c>
       <c r="C52" s="28" t="s">
-        <v>79</v>
+        <v>128</v>
       </c>
       <c r="D52" s="24" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="E52" s="20" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="F52" s="21">
         <v>45101</v>
@@ -2919,23 +3047,23 @@
       <c r="H52" s="22">
         <v>0</v>
       </c>
-      <c r="I52" s="72"/>
+      <c r="I52" s="79"/>
       <c r="J52" s="26"/>
       <c r="K52" s="2"/>
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1">
       <c r="A53" s="11"/>
       <c r="B53" s="47" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C53" s="28" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="E53" s="20" t="s">
-        <v>37</v>
+        <v>175</v>
       </c>
       <c r="F53" s="21">
         <v>45103</v>
@@ -2946,28 +3074,28 @@
       <c r="H53" s="22">
         <v>0</v>
       </c>
-      <c r="I53" s="71" t="s">
-        <v>165</v>
+      <c r="I53" s="78" t="s">
+        <v>176</v>
       </c>
       <c r="J53" s="26"/>
       <c r="K53" s="2"/>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1">
       <c r="A54" s="11"/>
-      <c r="B54" s="50" t="s">
-        <v>166</v>
-      </c>
-      <c r="C54" s="51" t="s">
-        <v>167</v>
+      <c r="B54" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="C54" s="28" t="s">
+        <v>178</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>168</v>
+        <v>179</v>
       </c>
       <c r="E54" s="20" t="s">
-        <v>169</v>
+        <v>138</v>
       </c>
       <c r="F54" s="21">
-        <v>45105</v>
+        <v>45103</v>
       </c>
       <c r="G54" s="21">
         <v>45107</v>
@@ -2975,45 +3103,67 @@
       <c r="H54" s="22">
         <v>0</v>
       </c>
-      <c r="I54" s="72"/>
+      <c r="I54" s="79"/>
       <c r="J54" s="26"/>
       <c r="K54" s="2"/>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1">
-      <c r="A55" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="B55" s="52" t="s">
-        <v>171</v>
-      </c>
-      <c r="C55" s="53"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="55"/>
-      <c r="F55" s="56">
+      <c r="A55" s="11"/>
+      <c r="B55" s="50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C55" s="51" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>182</v>
+      </c>
+      <c r="E55" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F55" s="21">
+        <v>45103</v>
+      </c>
+      <c r="G55" s="21">
+        <v>45107</v>
+      </c>
+      <c r="H55" s="22">
+        <v>0</v>
+      </c>
+      <c r="I55" s="79"/>
+      <c r="J55" s="26"/>
+      <c r="K55" s="2"/>
+    </row>
+    <row r="56" spans="1:11" ht="15.75" customHeight="1">
+      <c r="A56" s="11" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="C56" s="53"/>
+      <c r="D56" s="54"/>
+      <c r="E56" s="55"/>
+      <c r="F56" s="56">
         <v>45078</v>
       </c>
-      <c r="G55" s="56">
+      <c r="G56" s="56">
         <v>45107</v>
       </c>
-      <c r="H55" s="57"/>
-      <c r="I55" s="72"/>
-    </row>
-    <row r="56" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B56" s="58"/>
-      <c r="C56" s="58"/>
-      <c r="D56" s="58"/>
-      <c r="E56" s="58"/>
-      <c r="F56" s="59"/>
-      <c r="G56" s="59"/>
-      <c r="H56" s="59"/>
+      <c r="H56" s="57"/>
+      <c r="I56" s="79"/>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1">
-      <c r="B57" s="60"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
+      <c r="B57" s="58"/>
+      <c r="C57" s="58"/>
+      <c r="D57" s="58"/>
+      <c r="E57" s="58"/>
+      <c r="F57" s="59"/>
+      <c r="G57" s="59"/>
+      <c r="H57" s="59"/>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1">
+      <c r="B58" s="60"/>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
       <c r="H58" s="4"/>
@@ -4003,7 +4153,11 @@
       <c r="G255" s="4"/>
       <c r="H255" s="4"/>
     </row>
-    <row r="256" spans="6:8" ht="15.75" customHeight="1"/>
+    <row r="256" spans="6:8" ht="15.75" customHeight="1">
+      <c r="F256" s="4"/>
+      <c r="G256" s="4"/>
+      <c r="H256" s="4"/>
+    </row>
     <row r="257" ht="15.75" customHeight="1"/>
     <row r="258" ht="15.75" customHeight="1"/>
     <row r="259" ht="15.75" customHeight="1"/>
@@ -4758,21 +4912,22 @@
     <row r="1008" ht="15.75" customHeight="1"/>
     <row r="1009" ht="15.75" customHeight="1"/>
     <row r="1010" ht="15.75" customHeight="1"/>
+    <row r="1011" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="I43:I49"/>
     <mergeCell ref="I50:I52"/>
-    <mergeCell ref="I53:I55"/>
+    <mergeCell ref="I53:I56"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="I12:I21"/>
     <mergeCell ref="I22:I23"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="I29:I36"/>
-    <mergeCell ref="I40:I42"/>
+    <mergeCell ref="I25:I27"/>
+    <mergeCell ref="I28:I35"/>
+    <mergeCell ref="I39:I42"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="Ruta del repositorio Github:  https://github.com/LuisBDev/Sistema-de-Gestion-de-Incidencias" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -4784,101 +4939,176 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A2:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="4" max="4" width="35.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="15" customHeight="1">
+      <c r="A2" s="61" t="s">
+        <v>186</v>
+      </c>
+      <c r="B2" s="62" t="s">
+        <v>187</v>
+      </c>
+      <c r="C2" s="62" t="s">
+        <v>188</v>
+      </c>
+      <c r="D2" s="62" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="15" customHeight="1">
+      <c r="A3" s="63" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" s="64">
+        <v>45024</v>
+      </c>
+      <c r="C3" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="66" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="15" customHeight="1">
+      <c r="A4" s="67">
+        <v>44927</v>
+      </c>
+      <c r="B4" s="64">
+        <v>45047</v>
+      </c>
+      <c r="C4" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="D4" s="66" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15" customHeight="1">
+      <c r="A5" s="67">
+        <v>44958</v>
+      </c>
+      <c r="B5" s="64">
+        <v>45047</v>
+      </c>
+      <c r="C5" s="65" t="s">
+        <v>191</v>
+      </c>
+      <c r="D5" s="66" t="s">
+        <v>194</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <dimension ref="B1:C992"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="38.140625" customWidth="1"/>
-    <col min="4" max="6" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.109375" customWidth="1"/>
+    <col min="4" max="6" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" customHeight="1"/>
     <row r="2" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B2" s="61" t="s">
-        <v>172</v>
+      <c r="B2" s="68" t="s">
+        <v>195</v>
       </c>
       <c r="C2" s="11"/>
     </row>
     <row r="3" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B3" s="76" t="s">
-        <v>173</v>
-      </c>
-      <c r="C3" s="75"/>
+      <c r="B3" s="83" t="s">
+        <v>196</v>
+      </c>
+      <c r="C3" s="82"/>
     </row>
     <row r="4" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B4" s="62" t="s">
-        <v>174</v>
-      </c>
-      <c r="C4" s="63" t="s">
-        <v>175</v>
+      <c r="B4" s="69" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="70" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B5" s="64" t="s">
-        <v>176</v>
-      </c>
-      <c r="C5" s="65" t="s">
-        <v>177</v>
+      <c r="B5" s="71" t="s">
+        <v>199</v>
+      </c>
+      <c r="C5" s="72" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B6" s="64" t="s">
-        <v>178</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>179</v>
+      <c r="B6" s="71" t="s">
+        <v>201</v>
+      </c>
+      <c r="C6" s="72" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B7" s="64" t="s">
-        <v>180</v>
-      </c>
-      <c r="C7" s="65" t="s">
-        <v>181</v>
+      <c r="B7" s="71" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="72" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B8" s="66" t="s">
-        <v>182</v>
-      </c>
-      <c r="C8" s="65" t="s">
-        <v>179</v>
+      <c r="B8" s="73" t="s">
+        <v>205</v>
+      </c>
+      <c r="C8" s="72" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B9" s="64" t="s">
-        <v>183</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>184</v>
+      <c r="B9" s="71" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" s="72" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B10" s="64" t="s">
-        <v>185</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>179</v>
+      <c r="B10" s="71" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" s="72" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B11" s="67" t="s">
-        <v>186</v>
-      </c>
-      <c r="C11" s="68" t="s">
-        <v>187</v>
+      <c r="B11" s="74" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" s="75" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B12" s="69" t="s">
-        <v>188</v>
-      </c>
-      <c r="C12" s="70" t="s">
-        <v>189</v>
+      <c r="B12" s="76" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="77" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Actualizando estado del cronograma del proyecto
</commit_message>
<xml_diff>
--- a/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
+++ b/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
@@ -4,8 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Cronograma #1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Control de Versiones" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="IntegrantesRoles" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="IntegrantesRoles" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Control de Versiones" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="227">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -316,13 +316,13 @@
     <t>Revisión, análisis y validación de los Requisitos y Especificaciones del Software</t>
   </si>
   <si>
-    <t>Documento de Especificación de Requisitos</t>
-  </si>
-  <si>
-    <t>SGI-DERE.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Justiniano/A, Soller/PB</t>
+    <t>Documento de Validación de Requisitos y Especificaciones</t>
+  </si>
+  <si>
+    <t>SGI-DVRE.DOCX</t>
+  </si>
+  <si>
+    <t>Durand/PB, Justiniano/A, Soller/PB</t>
   </si>
   <si>
     <t>S5 - S6</t>
@@ -367,7 +367,7 @@
     <t>SGI-DEUI2.PDF</t>
   </si>
   <si>
-    <t>Huarhua/UX,  Soller/PB, Del Aguila/QA</t>
+    <t>Huarhua/UX,  Soller/PB</t>
   </si>
   <si>
     <t>Verificar y Actualizar documento de Especificación de la Base de Datos</t>
@@ -391,7 +391,7 @@
     <t>Soller/PB, Canecillas/A, Balceda/PB, Huarhua/AS</t>
   </si>
   <si>
-    <t>Codificación Autenticación de Usuario (Registro)</t>
+    <t>Codificación Autenticación de Usuario</t>
   </si>
   <si>
     <t>Módulo de Autenticación de Usuario</t>
@@ -415,16 +415,25 @@
     <t>Balarezo/A, Justiniano/A, Canecillas/A, Durand/PB</t>
   </si>
   <si>
+    <t>Realizar Documento de Pruebas de Software Maestro</t>
+  </si>
+  <si>
+    <t>Documento de Pruebas de Software Maestro</t>
+  </si>
+  <si>
+    <t>SGI-DPSM.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA</t>
+  </si>
+  <si>
     <t>Realizar Pruebas de validación del Software</t>
   </si>
   <si>
     <t>Documento de Pruebas de validación del Software</t>
   </si>
   <si>
-    <t>SGI-DPVS.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB, Soller/PB</t>
+    <t>SGI-DPVS1.DOCX</t>
   </si>
   <si>
     <t>Realizar Análisis de la calidad del software</t>
@@ -433,174 +442,186 @@
     <t>Documento de Análisis de la calidad del software</t>
   </si>
   <si>
+    <t>SGI-DACS1.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Soller/PB,  Durand/PB</t>
+  </si>
+  <si>
+    <t>Reportar estado actual del software</t>
+  </si>
+  <si>
+    <t>Reporte del Desarrollo del Software</t>
+  </si>
+  <si>
+    <t>SGI-RDS1.DOCX</t>
+  </si>
+  <si>
+    <t>Balarezo/JP, Durand/PB, Huarhua/AS</t>
+  </si>
+  <si>
+    <t>S7</t>
+  </si>
+  <si>
+    <t>Reporte del Segundo Sprint</t>
+  </si>
+  <si>
+    <t>SGI-RSS.DOCX</t>
+  </si>
+  <si>
+    <t>Canecillas/A, Balceda/PB</t>
+  </si>
+  <si>
+    <t>Documentar Acta de finalización del Hito 2</t>
+  </si>
+  <si>
+    <t>Acta de Finalización Hito 2</t>
+  </si>
+  <si>
+    <t>SGI-AFH2.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Soller/PB, Justiniano/A</t>
+  </si>
+  <si>
+    <t>Carga de Linea Base 2</t>
+  </si>
+  <si>
+    <t>Linea base 2</t>
+  </si>
+  <si>
+    <t>Hito 2 - Fin del Sprint #2</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 7 del Software - Seguimiento de Incidencias</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 7</t>
+  </si>
+  <si>
+    <t>SGI-DER7.DOCX</t>
+  </si>
+  <si>
+    <t>Especificar Requerimiento 8 del Software - Generación de Reportes</t>
+  </si>
+  <si>
+    <t>Documento de Especificación de Requerimiento 8</t>
+  </si>
+  <si>
+    <t>SGI-DER8.DOCX</t>
+  </si>
+  <si>
+    <t>Justiniano/A</t>
+  </si>
+  <si>
+    <t>Codificación de Gestión de Roles</t>
+  </si>
+  <si>
+    <t>Documento de Gestión de Roles</t>
+  </si>
+  <si>
+    <t>SGI-DGR.DOCX</t>
+  </si>
+  <si>
+    <t>Justiniano/A, Del Aguila/QA, Balceda/PB</t>
+  </si>
+  <si>
+    <t>Codificación de Seguimiento de incidencias</t>
+  </si>
+  <si>
+    <t>Documento de Seguimiento de Incidencias</t>
+  </si>
+  <si>
+    <t>SGI-DSI.DOCX</t>
+  </si>
+  <si>
+    <t>Codificación de Asignación de Personal</t>
+  </si>
+  <si>
+    <t>Documento de Asignación de Personal</t>
+  </si>
+  <si>
+    <t>SGI-DAP.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Durand/PB, Balarezo/JP, Soller/PB</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>SGI-DEUI3.PDF</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>SGI-DEBD3.DOCX</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
+  </si>
+  <si>
+    <t>SGI-DAS2.DOCX</t>
+  </si>
+  <si>
+    <t>Huarhua/AS, Durand/PB</t>
+  </si>
+  <si>
+    <t>Generar documentación para el usuario</t>
+  </si>
+  <si>
+    <t>Manual de usuario</t>
+  </si>
+  <si>
+    <t>SGI-MU.DOCX</t>
+  </si>
+  <si>
+    <t>Soller/PB, Balceda/PB, Huarhua/UI, Del Aguila/QA</t>
+  </si>
+  <si>
+    <t>SGI-DPVS2.DOCX</t>
+  </si>
+  <si>
+    <t>S9</t>
+  </si>
+  <si>
+    <t>Documento de Análisis de Calidad del Software</t>
+  </si>
+  <si>
     <t>SGI-DACS2.DOCX</t>
   </si>
   <si>
-    <t>Del Aguila/QA, Soller/PB,  Durand/PB</t>
-  </si>
-  <si>
-    <t>Reportar estado actual del software</t>
-  </si>
-  <si>
-    <t>Reporte del Desarrollo del Software</t>
-  </si>
-  <si>
     <t>SGI-RDS2.DOCX</t>
   </si>
   <si>
     <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB</t>
   </si>
   <si>
-    <t>S7</t>
-  </si>
-  <si>
-    <t>Reporte del Segundo Sprint</t>
-  </si>
-  <si>
-    <t>SGI-RSS.DOCX</t>
-  </si>
-  <si>
-    <t>Balarezo/JP, Canecillas/A, Balceda/PB</t>
-  </si>
-  <si>
-    <t>Documentar Acta de finalización del Hito 2</t>
-  </si>
-  <si>
-    <t>Acta de Finalización Hito 2</t>
-  </si>
-  <si>
-    <t>SGI-AFH2.DOCX</t>
+    <t>Reporte del Tercer Sprint</t>
+  </si>
+  <si>
+    <t>SGI-RTS.DOCX</t>
+  </si>
+  <si>
+    <t>Del Aguila/QA, Justiniano/A, Huarhua/AS</t>
+  </si>
+  <si>
+    <t>S9 - S10</t>
+  </si>
+  <si>
+    <t>Documentar Acta de finalización del Hito 3</t>
+  </si>
+  <si>
+    <t>Acta de Finalización Hito 3</t>
+  </si>
+  <si>
+    <t>SGI-AFH3.DOCX</t>
   </si>
   <si>
     <t>Balarezo/JP, Del Aguila/QA, Soller/PB</t>
   </si>
   <si>
-    <t>Carga de Linea Base 2</t>
-  </si>
-  <si>
-    <t>Linea base 2</t>
-  </si>
-  <si>
-    <t>Hito 2 - Fin del Sprint #2</t>
-  </si>
-  <si>
-    <t>Codificación asignación de personal encargado</t>
-  </si>
-  <si>
-    <t>Módulo de asignación de personal especializado</t>
-  </si>
-  <si>
-    <t>SGI-MAPE.DOCX</t>
-  </si>
-  <si>
-    <t>S7 -S8 - S9</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 7 del Software - Seguimiento de Incidencias</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 7</t>
-  </si>
-  <si>
-    <t>SGI-DER7.DOCX</t>
-  </si>
-  <si>
-    <t>Del Aguila/QA</t>
-  </si>
-  <si>
-    <t>Especificar Requerimiento 8 del Software - Generación de Reportes</t>
-  </si>
-  <si>
-    <t>Documento de Especificación de Requerimiento 8</t>
-  </si>
-  <si>
-    <t>SGI-DER8.DOCX</t>
-  </si>
-  <si>
-    <t>Justiniano/A</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar documento de Especificación de UI</t>
-  </si>
-  <si>
-    <t>SGI-DEUI3.PDF</t>
-  </si>
-  <si>
-    <t>Huarhua/UX,  Soller/PB</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
-    <t>SGI-DEBD3.DOCX</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
-  </si>
-  <si>
-    <t>SGI-DAS.DOCX</t>
-  </si>
-  <si>
-    <t>Huarhua/AS, Durand/PB</t>
-  </si>
-  <si>
-    <t>Generar documentación para el usuario</t>
-  </si>
-  <si>
-    <t>Manual de usuario</t>
-  </si>
-  <si>
-    <t>SGI-MU.DOCX</t>
-  </si>
-  <si>
-    <t>Soller/PB, Balceda/PB, Huarhua/UI, Del Aguila/QA</t>
-  </si>
-  <si>
-    <t>Realizar Pruebas de Seguridad del Software</t>
-  </si>
-  <si>
-    <t>Documento de Pruebas del Software</t>
-  </si>
-  <si>
-    <t>SGI-DPS.DOCX</t>
-  </si>
-  <si>
-    <t>Canecillas/A, Del Aguila/QA</t>
-  </si>
-  <si>
-    <t>S9</t>
-  </si>
-  <si>
-    <t>Documento de Análisis de Calidad del Software</t>
-  </si>
-  <si>
-    <t>SGI-DACS3.DOCX</t>
-  </si>
-  <si>
-    <t>SGI-RDS3.DOCX</t>
-  </si>
-  <si>
-    <t>Reporte del Tercer Sprint</t>
-  </si>
-  <si>
-    <t>SGI-RTS.DOCX</t>
-  </si>
-  <si>
-    <t>Del Aguila/QA, Justiniano/A, Huarhua/AS</t>
-  </si>
-  <si>
-    <t>S9 - S10</t>
-  </si>
-  <si>
-    <t>Documentar Acta de finalización del Hito 3</t>
-  </si>
-  <si>
-    <t>Acta de Finalización Hito 3</t>
-  </si>
-  <si>
-    <t>SGI-AFH3.DOCX</t>
-  </si>
-  <si>
     <t>Elaborar del acta de cierre del proyecto</t>
   </si>
   <si>
@@ -622,6 +643,60 @@
     <t>Hito 3 - Fin del Sprint #3</t>
   </si>
   <si>
+    <t xml:space="preserve">Herramienta: </t>
+  </si>
+  <si>
+    <t>GRUPO 5</t>
+  </si>
+  <si>
+    <t>Apellido y nombre</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Balarezo Ramos, Luis Jesús</t>
+  </si>
+  <si>
+    <t>Jefe de Proyecto / Analista Sr.</t>
+  </si>
+  <si>
+    <t>Durand Caracuzma,Marlon Milko</t>
+  </si>
+  <si>
+    <t>Programador Back-End</t>
+  </si>
+  <si>
+    <t>Del Aguila Febres,Brayan Tadeo</t>
+  </si>
+  <si>
+    <t>QA</t>
+  </si>
+  <si>
+    <t>Balceda Delgado, Mariana Alejandra</t>
+  </si>
+  <si>
+    <t>Canecillas Contreras,Juan Mariano</t>
+  </si>
+  <si>
+    <t>Analista Senior / DBA</t>
+  </si>
+  <si>
+    <t>Soller Barnechea,Carlos Javier</t>
+  </si>
+  <si>
+    <t>Huarhua Piñas Edson Sebastian</t>
+  </si>
+  <si>
+    <t>Diseñador UI UX / Arquitecto de software</t>
+  </si>
+  <si>
+    <t>Justiniano Quispe,Diego André</t>
+  </si>
+  <si>
+    <t>Analista Sr.</t>
+  </si>
+  <si>
     <t>Versión</t>
   </si>
   <si>
@@ -659,60 +734,6 @@
   </si>
   <si>
     <t>Plazos excesivos, por lo que se acortó el tiempo de entrega. / No se contaba con actividades de carga de LB.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Herramienta: </t>
-  </si>
-  <si>
-    <t>GRUPO 5</t>
-  </si>
-  <si>
-    <t>Apellido y nombre</t>
-  </si>
-  <si>
-    <t>Rol</t>
-  </si>
-  <si>
-    <t>Balarezo Ramos, Luis Jesús</t>
-  </si>
-  <si>
-    <t>Jefe de Proyecto / Analista Sr.</t>
-  </si>
-  <si>
-    <t>Durand Caracuzma,Marlon Milko</t>
-  </si>
-  <si>
-    <t>Programador Back-End</t>
-  </si>
-  <si>
-    <t>Del Aguila Febres,Brayan Tadeo</t>
-  </si>
-  <si>
-    <t>QA</t>
-  </si>
-  <si>
-    <t>Balceda Delgado, Mariana Alejandra</t>
-  </si>
-  <si>
-    <t>Canecillas Contreras,Juan Mariano</t>
-  </si>
-  <si>
-    <t>Analista Senior / DBA</t>
-  </si>
-  <si>
-    <t>Soller Barnechea,Carlos Javier</t>
-  </si>
-  <si>
-    <t>Huarhua Piñas Edson Sebastian</t>
-  </si>
-  <si>
-    <t>Diseñador UI UX / Arquitecto de software</t>
-  </si>
-  <si>
-    <t>Justiniano Quispe,Diego André</t>
-  </si>
-  <si>
-    <t>Analista Sr.</t>
   </si>
 </sst>
 </file>
@@ -880,17 +901,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Montserrat"/>
@@ -906,6 +916,17 @@
       <sz val="10.0"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="12">
@@ -1194,13 +1215,12 @@
       </bottom>
     </border>
     <border>
-      <left style="thin">
+      <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right style="medium">
+      <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
@@ -1264,6 +1284,28 @@
       </bottom>
     </border>
     <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1281,34 +1323,12 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
-      <left style="thick">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thick">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="95">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1431,18 +1451,15 @@
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="14" fillId="5" fontId="20" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="6" fontId="22" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="17" fillId="4" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="6" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="18" fillId="4" fontId="23" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="15" fillId="6" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="12" fillId="5" fontId="24" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="13" fillId="5" fontId="25" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1451,7 +1468,16 @@
     <xf borderId="14" fillId="5" fontId="25" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="11" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="18" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="16" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="16" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="11" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="11" fillId="10" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -1478,65 +1504,65 @@
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="13" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="13" fillId="11" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="1" fillId="5" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="3" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="16" fillId="11" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="16" fillId="11" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="28" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="28" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="25" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="28" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="28" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="5" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="3" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="4" fillId="3" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="3" fontId="27" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="4" fillId="4" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="4" fillId="4" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
     <xf borderId="3" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf borderId="26" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="24" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="27" fillId="4" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="25" fillId="4" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0"/>
     </xf>
     <xf borderId="5" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="6" fillId="4" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="6" fillId="4" fontId="29" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="13" fillId="11" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="16" fillId="11" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="16" fillId="11" fontId="30" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="26" fillId="0" fontId="31" numFmtId="4" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="27" fillId="0" fontId="31" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="27" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="27" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="26" fillId="0" fontId="31" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0"/>
+    </xf>
+    <xf borderId="26" fillId="0" fontId="31" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1765,7 +1791,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="15.88"/>
     <col customWidth="1" min="2" max="2" width="69.5"/>
-    <col customWidth="1" min="3" max="3" width="38.63"/>
+    <col customWidth="1" min="3" max="3" width="52.13"/>
     <col customWidth="1" min="4" max="4" width="21.25"/>
     <col customWidth="1" min="5" max="5" width="46.13"/>
     <col customWidth="1" min="6" max="7" width="13.25"/>
@@ -1942,7 +1968,7 @@
       </c>
       <c r="J11" s="5"/>
     </row>
-    <row r="12" ht="31.5" customHeight="1">
+    <row r="12" ht="22.5" customHeight="1">
       <c r="A12" s="15"/>
       <c r="B12" s="21" t="s">
         <v>23</v>
@@ -2382,14 +2408,16 @@
       <c r="G28" s="48">
         <v>45054.0</v>
       </c>
-      <c r="H28" s="49"/>
+      <c r="H28" s="49">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="15"/>
       <c r="B29" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="36" t="s">
+      <c r="C29" s="38" t="s">
         <v>87</v>
       </c>
       <c r="D29" s="32" t="s">
@@ -2405,7 +2433,7 @@
         <v>45057.0</v>
       </c>
       <c r="H29" s="51">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="I29" s="27" t="s">
         <v>90</v>
@@ -2433,8 +2461,8 @@
       <c r="G30" s="25">
         <v>45060.0</v>
       </c>
-      <c r="H30" s="26">
-        <v>0.0</v>
+      <c r="H30" s="33">
+        <v>1.0</v>
       </c>
       <c r="J30" s="34"/>
       <c r="K30" s="5"/>
@@ -2459,8 +2487,8 @@
       <c r="G31" s="25">
         <v>45063.0</v>
       </c>
-      <c r="H31" s="26">
-        <v>0.0</v>
+      <c r="H31" s="33">
+        <v>1.0</v>
       </c>
       <c r="J31" s="34"/>
       <c r="K31" s="5"/>
@@ -2485,8 +2513,8 @@
       <c r="G32" s="25">
         <v>45063.0</v>
       </c>
-      <c r="H32" s="26">
-        <v>0.0</v>
+      <c r="H32" s="33">
+        <v>1.0</v>
       </c>
       <c r="J32" s="34"/>
       <c r="K32" s="5"/>
@@ -2511,15 +2539,15 @@
       <c r="G33" s="25">
         <v>45063.0</v>
       </c>
-      <c r="H33" s="53">
-        <v>0.0</v>
+      <c r="H33" s="33">
+        <v>1.0</v>
       </c>
       <c r="J33" s="34"/>
       <c r="K33" s="5"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="15"/>
-      <c r="B34" s="54" t="s">
+      <c r="B34" s="53" t="s">
         <v>105</v>
       </c>
       <c r="C34" s="44" t="s">
@@ -2537,8 +2565,8 @@
       <c r="G34" s="25">
         <v>45063.0</v>
       </c>
-      <c r="H34" s="51">
-        <v>0.0</v>
+      <c r="H34" s="33">
+        <v>1.0</v>
       </c>
       <c r="J34" s="34"/>
       <c r="K34" s="5"/>
@@ -2563,8 +2591,8 @@
       <c r="G35" s="25">
         <v>45070.0</v>
       </c>
-      <c r="H35" s="53">
-        <v>0.0</v>
+      <c r="H35" s="33">
+        <v>1.0</v>
       </c>
       <c r="J35" s="34"/>
       <c r="K35" s="5"/>
@@ -2589,8 +2617,8 @@
       <c r="G36" s="25">
         <v>45070.0</v>
       </c>
-      <c r="H36" s="53">
-        <v>0.0</v>
+      <c r="H36" s="33">
+        <v>1.0</v>
       </c>
       <c r="J36" s="34"/>
       <c r="K36" s="5"/>
@@ -2615,14 +2643,14 @@
       <c r="G37" s="25">
         <v>45070.0</v>
       </c>
-      <c r="H37" s="53">
-        <v>0.0</v>
+      <c r="H37" s="33">
+        <v>1.0</v>
       </c>
       <c r="I37" s="27"/>
       <c r="J37" s="34"/>
       <c r="K37" s="5"/>
     </row>
-    <row r="38" ht="24.75" customHeight="1">
+    <row r="38" ht="21.75" customHeight="1">
       <c r="A38" s="15"/>
       <c r="B38" s="37" t="s">
         <v>120</v>
@@ -2642,14 +2670,14 @@
       <c r="G38" s="25">
         <v>45077.0</v>
       </c>
-      <c r="H38" s="53">
-        <v>0.0</v>
+      <c r="H38" s="33">
+        <v>1.0</v>
       </c>
       <c r="I38" s="27"/>
       <c r="J38" s="34"/>
       <c r="K38" s="5"/>
     </row>
-    <row r="39" ht="15.75" customHeight="1">
+    <row r="39" ht="24.75" customHeight="1">
       <c r="A39" s="15"/>
       <c r="B39" s="37" t="s">
         <v>124</v>
@@ -2661,7 +2689,7 @@
         <v>126</v>
       </c>
       <c r="E39" s="24" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="F39" s="25">
         <v>45060.0</v>
@@ -2669,8 +2697,8 @@
       <c r="G39" s="25">
         <v>45077.0</v>
       </c>
-      <c r="H39" s="53">
-        <v>0.0</v>
+      <c r="H39" s="33">
+        <v>1.0</v>
       </c>
       <c r="I39" s="27"/>
       <c r="J39" s="34"/>
@@ -2678,17 +2706,17 @@
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="15"/>
-      <c r="B40" s="21" t="s">
+      <c r="B40" s="37" t="s">
+        <v>127</v>
+      </c>
+      <c r="C40" s="38" t="s">
         <v>128</v>
       </c>
-      <c r="C40" s="36" t="s">
+      <c r="D40" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="32" t="s">
+      <c r="E40" s="24" t="s">
         <v>130</v>
-      </c>
-      <c r="E40" s="24" t="s">
-        <v>131</v>
       </c>
       <c r="F40" s="25">
         <v>45060.0</v>
@@ -2696,28 +2724,26 @@
       <c r="G40" s="25">
         <v>45077.0</v>
       </c>
-      <c r="H40" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="I40" s="27" t="s">
-        <v>132</v>
-      </c>
+      <c r="H40" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="I40" s="27"/>
       <c r="J40" s="34"/>
       <c r="K40" s="5"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="15"/>
       <c r="B41" s="21" t="s">
-        <v>75</v>
+        <v>131</v>
       </c>
       <c r="C41" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D41" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="D41" s="32" t="s">
+      <c r="E41" s="24" t="s">
         <v>134</v>
-      </c>
-      <c r="E41" s="24" t="s">
-        <v>135</v>
       </c>
       <c r="F41" s="25">
         <v>45060.0</v>
@@ -2725,25 +2751,28 @@
       <c r="G41" s="25">
         <v>45077.0</v>
       </c>
-      <c r="H41" s="26">
-        <v>0.0</v>
+      <c r="H41" s="33">
+        <v>1.0</v>
+      </c>
+      <c r="I41" s="27" t="s">
+        <v>135</v>
       </c>
       <c r="J41" s="34"/>
       <c r="K41" s="5"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="15"/>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="C42" s="38" t="s">
+      <c r="D42" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="D42" s="32" t="s">
+      <c r="E42" s="24" t="s">
         <v>138</v>
-      </c>
-      <c r="E42" s="24" t="s">
-        <v>139</v>
       </c>
       <c r="F42" s="25">
         <v>45060.0</v>
@@ -2751,8 +2780,8 @@
       <c r="G42" s="25">
         <v>45077.0</v>
       </c>
-      <c r="H42" s="26">
-        <v>0.0</v>
+      <c r="H42" s="33">
+        <v>1.0</v>
       </c>
       <c r="J42" s="34"/>
       <c r="K42" s="5"/>
@@ -2760,16 +2789,16 @@
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="15"/>
       <c r="B43" s="37" t="s">
+        <v>139</v>
+      </c>
+      <c r="C43" s="38" t="s">
         <v>140</v>
       </c>
-      <c r="C43" s="38" t="s">
-        <v>21</v>
-      </c>
       <c r="D43" s="32" t="s">
-        <v>21</v>
+        <v>141</v>
       </c>
       <c r="E43" s="24" t="s">
-        <v>34</v>
+        <v>142</v>
       </c>
       <c r="F43" s="25">
         <v>45060.0</v>
@@ -2778,69 +2807,66 @@
         <v>45077.0</v>
       </c>
       <c r="H43" s="33">
-        <v>0.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="J43" s="34"/>
+      <c r="K43" s="5"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="15" t="s">
-        <v>141</v>
-      </c>
-      <c r="B44" s="45" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" s="55"/>
-      <c r="D44" s="56"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="48">
+      <c r="A44" s="15"/>
+      <c r="B44" s="37" t="s">
+        <v>143</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D44" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44" s="25">
+        <v>45060.0</v>
+      </c>
+      <c r="G44" s="25">
+        <v>45077.0</v>
+      </c>
+      <c r="H44" s="33">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="45" ht="15.75" customHeight="1">
+      <c r="A45" s="15" t="s">
+        <v>144</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="C45" s="54"/>
+      <c r="D45" s="55"/>
+      <c r="E45" s="55"/>
+      <c r="F45" s="48">
         <v>45051.0</v>
       </c>
-      <c r="G44" s="48">
+      <c r="G45" s="48">
         <v>45077.0</v>
       </c>
-      <c r="H44" s="57"/>
-    </row>
-    <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="15"/>
-      <c r="B45" s="58" t="s">
-        <v>143</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>144</v>
-      </c>
-      <c r="D45" s="32" t="s">
-        <v>145</v>
-      </c>
-      <c r="E45" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="F45" s="25">
-        <v>45078.0</v>
-      </c>
-      <c r="G45" s="25">
-        <v>45092.0</v>
-      </c>
-      <c r="H45" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="I45" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="J45" s="34"/>
-      <c r="K45" s="5"/>
+      <c r="H45" s="56"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="15"/>
       <c r="B46" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="38" t="s">
         <v>147</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="D46" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="D46" s="32" t="s">
-        <v>149</v>
-      </c>
       <c r="E46" s="24" t="s">
-        <v>150</v>
+        <v>123</v>
       </c>
       <c r="F46" s="25">
         <v>45078.0</v>
@@ -2851,22 +2877,23 @@
       <c r="H46" s="26">
         <v>0.0</v>
       </c>
+      <c r="I46" s="27"/>
       <c r="J46" s="34"/>
       <c r="K46" s="5"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="15"/>
       <c r="B47" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="C47" s="40" t="s">
+        <v>150</v>
+      </c>
+      <c r="D47" s="41" t="s">
         <v>151</v>
       </c>
-      <c r="C47" s="40" t="s">
+      <c r="E47" s="42" t="s">
         <v>152</v>
-      </c>
-      <c r="D47" s="41" t="s">
-        <v>153</v>
-      </c>
-      <c r="E47" s="42" t="s">
-        <v>154</v>
       </c>
       <c r="F47" s="25">
         <v>45078.0</v>
@@ -2882,20 +2909,20 @@
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="15"/>
-      <c r="B48" s="59" t="s">
+      <c r="B48" s="57" t="s">
+        <v>153</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>154</v>
+      </c>
+      <c r="D48" s="58" t="s">
         <v>155</v>
       </c>
-      <c r="C48" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="32" t="s">
+      <c r="E48" s="59" t="s">
         <v>156</v>
       </c>
-      <c r="E48" s="24" t="s">
-        <v>157</v>
-      </c>
       <c r="F48" s="25">
-        <v>45080.0</v>
+        <v>45078.0</v>
       </c>
       <c r="G48" s="25">
         <v>45092.0</v>
@@ -2909,19 +2936,19 @@
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="15"/>
       <c r="B49" s="60" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="38" t="s">
         <v>158</v>
-      </c>
-      <c r="C49" s="44" t="s">
-        <v>67</v>
       </c>
       <c r="D49" s="32" t="s">
         <v>159</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
       <c r="F49" s="25">
-        <v>45080.0</v>
+        <v>45078.0</v>
       </c>
       <c r="G49" s="25">
         <v>45092.0</v>
@@ -2934,23 +2961,23 @@
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="15"/>
-      <c r="B50" s="61" t="s">
+      <c r="B50" s="60" t="s">
         <v>160</v>
       </c>
-      <c r="C50" s="36" t="s">
-        <v>71</v>
+      <c r="C50" s="38" t="s">
+        <v>161</v>
       </c>
       <c r="D50" s="32" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="E50" s="24" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="F50" s="25">
-        <v>45081.0</v>
+        <v>45078.0</v>
       </c>
       <c r="G50" s="25">
-        <v>45097.0</v>
+        <v>45092.0</v>
       </c>
       <c r="H50" s="26">
         <v>0.0</v>
@@ -2958,25 +2985,25 @@
       <c r="J50" s="34"/>
       <c r="K50" s="5"/>
     </row>
-    <row r="51" ht="14.25" customHeight="1">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="15"/>
       <c r="B51" s="61" t="s">
-        <v>163</v>
-      </c>
-      <c r="C51" s="36" t="s">
         <v>164</v>
+      </c>
+      <c r="C51" s="44" t="s">
+        <v>62</v>
       </c>
       <c r="D51" s="32" t="s">
         <v>165</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>166</v>
+        <v>104</v>
       </c>
       <c r="F51" s="25">
-        <v>45086.0</v>
+        <v>45080.0</v>
       </c>
       <c r="G51" s="25">
-        <v>45097.0</v>
+        <v>45092.0</v>
       </c>
       <c r="H51" s="26">
         <v>0.0</v>
@@ -2986,52 +3013,49 @@
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="15"/>
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="62" t="s">
+        <v>166</v>
+      </c>
+      <c r="C52" s="44" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="32" t="s">
         <v>167</v>
       </c>
-      <c r="C52" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="D52" s="32" t="s">
-        <v>169</v>
-      </c>
       <c r="E52" s="24" t="s">
-        <v>170</v>
+        <v>69</v>
       </c>
       <c r="F52" s="25">
-        <v>45097.0</v>
+        <v>45080.0</v>
       </c>
       <c r="G52" s="25">
-        <v>45101.0</v>
+        <v>45092.0</v>
       </c>
       <c r="H52" s="26">
         <v>0.0</v>
       </c>
-      <c r="I52" s="27" t="s">
-        <v>171</v>
-      </c>
       <c r="J52" s="34"/>
       <c r="K52" s="5"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="15"/>
-      <c r="B53" s="37" t="s">
-        <v>124</v>
-      </c>
-      <c r="C53" s="38" t="s">
-        <v>172</v>
+      <c r="B53" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="C53" s="36" t="s">
+        <v>71</v>
       </c>
       <c r="D53" s="32" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="E53" s="24" t="s">
-        <v>53</v>
+        <v>170</v>
       </c>
       <c r="F53" s="25">
-        <v>45101.0</v>
+        <v>45081.0</v>
       </c>
       <c r="G53" s="25">
-        <v>45107.0</v>
+        <v>45097.0</v>
       </c>
       <c r="H53" s="26">
         <v>0.0</v>
@@ -3039,25 +3063,25 @@
       <c r="J53" s="34"/>
       <c r="K53" s="5"/>
     </row>
-    <row r="54" ht="15.75" customHeight="1">
+    <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="15"/>
-      <c r="B54" s="61" t="s">
-        <v>128</v>
+      <c r="B54" s="63" t="s">
+        <v>171</v>
       </c>
       <c r="C54" s="36" t="s">
-        <v>129</v>
+        <v>172</v>
       </c>
       <c r="D54" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="E54" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="E54" s="24" t="s">
-        <v>131</v>
-      </c>
       <c r="F54" s="25">
-        <v>45101.0</v>
+        <v>45086.0</v>
       </c>
       <c r="G54" s="25">
-        <v>45107.0</v>
+        <v>45097.0</v>
       </c>
       <c r="H54" s="26">
         <v>0.0</v>
@@ -3067,29 +3091,29 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="15"/>
-      <c r="B55" s="61" t="s">
-        <v>75</v>
-      </c>
-      <c r="C55" s="36" t="s">
+      <c r="B55" s="37" t="s">
+        <v>124</v>
+      </c>
+      <c r="C55" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="D55" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="D55" s="32" t="s">
-        <v>176</v>
-      </c>
       <c r="E55" s="24" t="s">
-        <v>177</v>
+        <v>123</v>
       </c>
       <c r="F55" s="25">
-        <v>45103.0</v>
+        <v>45097.0</v>
       </c>
       <c r="G55" s="25">
-        <v>45107.0</v>
+        <v>45101.0</v>
       </c>
       <c r="H55" s="26">
         <v>0.0</v>
       </c>
       <c r="I55" s="27" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="J55" s="34"/>
       <c r="K55" s="5"/>
@@ -3097,19 +3121,19 @@
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="15"/>
       <c r="B56" s="37" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="C56" s="38" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D56" s="32" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="E56" s="24" t="s">
-        <v>139</v>
+        <v>53</v>
       </c>
       <c r="F56" s="25">
-        <v>45103.0</v>
+        <v>45101.0</v>
       </c>
       <c r="G56" s="25">
         <v>45107.0</v>
@@ -3122,20 +3146,20 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="15"/>
-      <c r="B57" s="62" t="s">
-        <v>182</v>
-      </c>
-      <c r="C57" s="63" t="s">
-        <v>183</v>
+      <c r="B57" s="63" t="s">
+        <v>131</v>
+      </c>
+      <c r="C57" s="36" t="s">
+        <v>132</v>
       </c>
       <c r="D57" s="32" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E57" s="24" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="F57" s="25">
-        <v>45103.0</v>
+        <v>45101.0</v>
       </c>
       <c r="G57" s="25">
         <v>45107.0</v>
@@ -3148,17 +3172,17 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="15"/>
-      <c r="B58" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="C58" s="38" t="s">
-        <v>21</v>
+      <c r="B58" s="63" t="s">
+        <v>75</v>
+      </c>
+      <c r="C58" s="36" t="s">
+        <v>181</v>
       </c>
       <c r="D58" s="32" t="s">
-        <v>21</v>
+        <v>182</v>
       </c>
       <c r="E58" s="24" t="s">
-        <v>34</v>
+        <v>183</v>
       </c>
       <c r="F58" s="25">
         <v>45103.0</v>
@@ -3166,54 +3190,120 @@
       <c r="G58" s="25">
         <v>45107.0</v>
       </c>
-      <c r="H58" s="33">
+      <c r="H58" s="26">
         <v>0.0</v>
       </c>
+      <c r="I58" s="27" t="s">
+        <v>184</v>
+      </c>
+      <c r="J58" s="34"/>
+      <c r="K58" s="5"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="15"/>
+      <c r="B59" s="37" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>186</v>
+      </c>
+      <c r="D59" s="32" t="s">
         <v>187</v>
       </c>
-      <c r="B59" s="64" t="s">
+      <c r="E59" s="24" t="s">
         <v>188</v>
       </c>
-      <c r="C59" s="65"/>
-      <c r="D59" s="66"/>
-      <c r="E59" s="67"/>
-      <c r="F59" s="68">
+      <c r="F59" s="25">
+        <v>45103.0</v>
+      </c>
+      <c r="G59" s="25">
+        <v>45107.0</v>
+      </c>
+      <c r="H59" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="J59" s="34"/>
+      <c r="K59" s="5"/>
+    </row>
+    <row r="60" ht="15.75" customHeight="1">
+      <c r="A60" s="15"/>
+      <c r="B60" s="64" t="s">
+        <v>189</v>
+      </c>
+      <c r="C60" s="65" t="s">
+        <v>190</v>
+      </c>
+      <c r="D60" s="32" t="s">
+        <v>191</v>
+      </c>
+      <c r="E60" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="F60" s="25">
+        <v>45103.0</v>
+      </c>
+      <c r="G60" s="25">
+        <v>45107.0</v>
+      </c>
+      <c r="H60" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="J60" s="34"/>
+      <c r="K60" s="5"/>
+    </row>
+    <row r="61" ht="15.75" customHeight="1">
+      <c r="A61" s="15"/>
+      <c r="B61" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="C61" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D61" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E61" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F61" s="25">
+        <v>45103.0</v>
+      </c>
+      <c r="G61" s="25">
+        <v>45107.0</v>
+      </c>
+      <c r="H61" s="33">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="62" ht="15.75" customHeight="1">
+      <c r="A62" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="B62" s="66" t="s">
+        <v>195</v>
+      </c>
+      <c r="C62" s="67"/>
+      <c r="D62" s="68"/>
+      <c r="E62" s="69"/>
+      <c r="F62" s="70">
         <v>45078.0</v>
       </c>
-      <c r="G59" s="68">
+      <c r="G62" s="70">
         <v>45107.0</v>
       </c>
-      <c r="H59" s="69"/>
-    </row>
-    <row r="60" ht="15.75" customHeight="1">
-      <c r="B60" s="70"/>
-      <c r="C60" s="70"/>
-      <c r="D60" s="70"/>
-      <c r="E60" s="70"/>
-      <c r="F60" s="71"/>
-      <c r="G60" s="71"/>
-      <c r="H60" s="71"/>
-    </row>
-    <row r="61" ht="15.75" customHeight="1">
-      <c r="B61" s="72"/>
-      <c r="F61" s="7"/>
-      <c r="G61" s="7"/>
-      <c r="H61" s="7"/>
-    </row>
-    <row r="62" ht="15.75" customHeight="1">
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
+      <c r="H62" s="71"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="F63" s="7"/>
-      <c r="G63" s="7"/>
-      <c r="H63" s="7"/>
+      <c r="B63" s="72"/>
+      <c r="C63" s="72"/>
+      <c r="D63" s="72"/>
+      <c r="E63" s="72"/>
+      <c r="F63" s="73"/>
+      <c r="G63" s="73"/>
+      <c r="H63" s="73"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
+      <c r="B64" s="74"/>
       <c r="F64" s="7"/>
       <c r="G64" s="7"/>
       <c r="H64" s="7"/>
@@ -4193,9 +4283,21 @@
       <c r="G259" s="7"/>
       <c r="H259" s="7"/>
     </row>
-    <row r="260" ht="15.75" customHeight="1"/>
-    <row r="261" ht="15.75" customHeight="1"/>
-    <row r="262" ht="15.75" customHeight="1"/>
+    <row r="260" ht="15.75" customHeight="1">
+      <c r="F260" s="7"/>
+      <c r="G260" s="7"/>
+      <c r="H260" s="7"/>
+    </row>
+    <row r="261" ht="15.75" customHeight="1">
+      <c r="F261" s="7"/>
+      <c r="G261" s="7"/>
+      <c r="H261" s="7"/>
+    </row>
+    <row r="262" ht="15.75" customHeight="1">
+      <c r="F262" s="7"/>
+      <c r="G262" s="7"/>
+      <c r="H262" s="7"/>
+    </row>
     <row r="263" ht="15.75" customHeight="1"/>
     <row r="264" ht="15.75" customHeight="1"/>
     <row r="265" ht="15.75" customHeight="1"/>
@@ -4948,18 +5050,21 @@
     <row r="1012" ht="15.75" customHeight="1"/>
     <row r="1013" ht="15.75" customHeight="1"/>
     <row r="1014" ht="15.75" customHeight="1"/>
+    <row r="1015" ht="15.75" customHeight="1"/>
+    <row r="1016" ht="15.75" customHeight="1"/>
+    <row r="1017" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="I45:I51"/>
-    <mergeCell ref="I52:I54"/>
-    <mergeCell ref="I55:I59"/>
+    <mergeCell ref="I58:I62"/>
+    <mergeCell ref="I46:I54"/>
+    <mergeCell ref="I55:I57"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="I12:I21"/>
     <mergeCell ref="I22:I23"/>
+    <mergeCell ref="I25:I28"/>
     <mergeCell ref="I29:I36"/>
-    <mergeCell ref="I25:I28"/>
-    <mergeCell ref="I40:I44"/>
+    <mergeCell ref="I41:I45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="B2"/>
@@ -4972,110 +5077,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="4" max="4" width="35.5"/>
-    <col customWidth="1" min="5" max="5" width="29.88"/>
-  </cols>
-  <sheetData>
-    <row r="2">
-      <c r="A2" s="73" t="s">
-        <v>189</v>
-      </c>
-      <c r="B2" s="74" t="s">
-        <v>190</v>
-      </c>
-      <c r="C2" s="74" t="s">
-        <v>191</v>
-      </c>
-      <c r="D2" s="74" t="s">
-        <v>192</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="B3" s="77">
-        <v>45024.0</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>195</v>
-      </c>
-      <c r="D3" s="79" t="s">
-        <v>196</v>
-      </c>
-      <c r="E3" s="78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="80">
-        <v>44927.0</v>
-      </c>
-      <c r="B4" s="77">
-        <v>45047.0</v>
-      </c>
-      <c r="C4" s="78" t="s">
-        <v>195</v>
-      </c>
-      <c r="D4" s="79" t="s">
-        <v>197</v>
-      </c>
-      <c r="E4" s="78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="80">
-        <v>44958.0</v>
-      </c>
-      <c r="B5" s="77">
-        <v>45047.0</v>
-      </c>
-      <c r="C5" s="78" t="s">
-        <v>195</v>
-      </c>
-      <c r="D5" s="79" t="s">
-        <v>198</v>
-      </c>
-      <c r="E5" s="78" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="81" t="s">
-        <v>199</v>
-      </c>
-      <c r="B6" s="77">
-        <v>45053.0</v>
-      </c>
-      <c r="C6" s="78" t="s">
-        <v>195</v>
-      </c>
-      <c r="D6" s="79" t="s">
-        <v>200</v>
-      </c>
-      <c r="E6" s="79" t="s">
-        <v>201</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -5094,87 +5095,87 @@
   <sheetData>
     <row r="1" ht="15.75" customHeight="1"/>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="B2" s="82" t="s">
+      <c r="B2" s="75" t="s">
+        <v>196</v>
+      </c>
+      <c r="C2" s="15"/>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="B3" s="76" t="s">
+        <v>197</v>
+      </c>
+      <c r="C3" s="4"/>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="B4" s="77" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="78" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="B5" s="79" t="s">
+        <v>200</v>
+      </c>
+      <c r="C5" s="80" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="B6" s="79" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="15"/>
-    </row>
-    <row r="3" ht="15.75" customHeight="1">
-      <c r="B3" s="83" t="s">
+      <c r="C6" s="80" t="s">
         <v>203</v>
       </c>
-      <c r="C3" s="4"/>
-    </row>
-    <row r="4" ht="15.75" customHeight="1">
-      <c r="B4" s="84" t="s">
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="B7" s="79" t="s">
         <v>204</v>
       </c>
-      <c r="C4" s="85" t="s">
+      <c r="C7" s="80" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="5" ht="15.75" customHeight="1">
-      <c r="B5" s="86" t="s">
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="B8" s="81" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="87" t="s">
+      <c r="C8" s="80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="B9" s="79" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="6" ht="15.75" customHeight="1">
-      <c r="B6" s="86" t="s">
+      <c r="C9" s="80" t="s">
         <v>208</v>
       </c>
-      <c r="C6" s="87" t="s">
+    </row>
+    <row r="10" ht="15.75" customHeight="1">
+      <c r="B10" s="79" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="7" ht="15.75" customHeight="1">
-      <c r="B7" s="86" t="s">
+      <c r="C10" s="80" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="11" ht="15.75" customHeight="1">
+      <c r="B11" s="82" t="s">
         <v>210</v>
       </c>
-      <c r="C7" s="87" t="s">
+      <c r="C11" s="83" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="8" ht="15.75" customHeight="1">
-      <c r="B8" s="88" t="s">
+    <row r="12" ht="15.75" customHeight="1">
+      <c r="B12" s="84" t="s">
         <v>212</v>
       </c>
-      <c r="C8" s="87" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="9" ht="15.75" customHeight="1">
-      <c r="B9" s="86" t="s">
+      <c r="C12" s="85" t="s">
         <v>213</v>
-      </c>
-      <c r="C9" s="87" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="10" ht="15.75" customHeight="1">
-      <c r="B10" s="86" t="s">
-        <v>215</v>
-      </c>
-      <c r="C10" s="87" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="11" ht="15.75" customHeight="1">
-      <c r="B11" s="89" t="s">
-        <v>216</v>
-      </c>
-      <c r="C11" s="90" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="B12" s="91" t="s">
-        <v>218</v>
-      </c>
-      <c r="C12" s="92" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1"/>
@@ -6166,4 +6167,108 @@
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <cols>
+    <col customWidth="1" min="4" max="4" width="35.5"/>
+    <col customWidth="1" min="5" max="5" width="29.88"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="86" t="s">
+        <v>214</v>
+      </c>
+      <c r="B2" s="87" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="87" t="s">
+        <v>216</v>
+      </c>
+      <c r="D2" s="87" t="s">
+        <v>217</v>
+      </c>
+      <c r="E2" s="88" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="89" t="s">
+        <v>219</v>
+      </c>
+      <c r="B3" s="90">
+        <v>45024.0</v>
+      </c>
+      <c r="C3" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D3" s="92" t="s">
+        <v>221</v>
+      </c>
+      <c r="E3" s="91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="93">
+        <v>44927.0</v>
+      </c>
+      <c r="B4" s="90">
+        <v>45047.0</v>
+      </c>
+      <c r="C4" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" s="92" t="s">
+        <v>222</v>
+      </c>
+      <c r="E4" s="91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="93">
+        <v>44958.0</v>
+      </c>
+      <c r="B5" s="90">
+        <v>45047.0</v>
+      </c>
+      <c r="C5" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D5" s="92" t="s">
+        <v>223</v>
+      </c>
+      <c r="E5" s="91" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="94" t="s">
+        <v>224</v>
+      </c>
+      <c r="B6" s="90">
+        <v>45053.0</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D6" s="92" t="s">
+        <v>225</v>
+      </c>
+      <c r="E6" s="92" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion avance del cronograma del proyecto
</commit_message>
<xml_diff>
--- a/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
+++ b/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="228">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -514,6 +514,18 @@
     <t>Justiniano/A</t>
   </si>
   <si>
+    <t>Verificar y finalizar documento de Especificación de UI</t>
+  </si>
+  <si>
+    <t>SGI-DEUI3.PDF</t>
+  </si>
+  <si>
+    <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
+  </si>
+  <si>
+    <t>SGI-DEBD3.DOCX</t>
+  </si>
+  <si>
     <t>Codificación de Gestión de Roles</t>
   </si>
   <si>
@@ -547,18 +559,6 @@
     <t>Del Aguila/QA, Durand/PB, Balarezo/JP, Soller/PB</t>
   </si>
   <si>
-    <t>Verificar y finalizar documento de Especificación de UI</t>
-  </si>
-  <si>
-    <t>SGI-DEUI3.PDF</t>
-  </si>
-  <si>
-    <t>Verificar y finalizar documento de Especificación de la Base de Datos</t>
-  </si>
-  <si>
-    <t>SGI-DEBD3.DOCX</t>
-  </si>
-  <si>
     <t>Verificar y finalizar la Arquitectura y Diseño del Software</t>
   </si>
   <si>
@@ -734,6 +734,9 @@
   </si>
   <si>
     <t>Plazos excesivos, por lo que se acortó el tiempo de entrega. / No se contaba con actividades de carga de LB.</t>
+  </si>
+  <si>
+    <t>Actualización del avance de los ítems al 100%</t>
   </si>
 </sst>
 </file>
@@ -1468,7 +1471,9 @@
     <xf borderId="14" fillId="5" fontId="25" numFmtId="9" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="18" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+    <xf borderId="11" fillId="10" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="15" fillId="10" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="18" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="16" fillId="4" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
@@ -1480,8 +1485,6 @@
     <xf borderId="11" fillId="10" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="11" fillId="10" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="10" fontId="22" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="11" fillId="10" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="15" fillId="10" fontId="10" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="19" fillId="4" fontId="11" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
@@ -2874,8 +2877,8 @@
       <c r="G46" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H46" s="26">
-        <v>0.0</v>
+      <c r="H46" s="33">
+        <v>1.0</v>
       </c>
       <c r="I46" s="27"/>
       <c r="J46" s="34"/>
@@ -2901,8 +2904,8 @@
       <c r="G47" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H47" s="26">
-        <v>0.0</v>
+      <c r="H47" s="33">
+        <v>1.0</v>
       </c>
       <c r="J47" s="34"/>
       <c r="K47" s="5"/>
@@ -2912,66 +2915,66 @@
       <c r="B48" s="57" t="s">
         <v>153</v>
       </c>
-      <c r="C48" s="38" t="s">
+      <c r="C48" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="D48" s="32" t="s">
         <v>154</v>
       </c>
-      <c r="D48" s="58" t="s">
-        <v>155</v>
-      </c>
-      <c r="E48" s="59" t="s">
-        <v>156</v>
+      <c r="E48" s="24" t="s">
+        <v>104</v>
       </c>
       <c r="F48" s="25">
-        <v>45078.0</v>
+        <v>45080.0</v>
       </c>
       <c r="G48" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H48" s="26">
-        <v>0.0</v>
+      <c r="H48" s="33">
+        <v>1.0</v>
       </c>
       <c r="J48" s="34"/>
       <c r="K48" s="5"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="15"/>
-      <c r="B49" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C49" s="38" t="s">
-        <v>158</v>
+      <c r="B49" s="58" t="s">
+        <v>155</v>
+      </c>
+      <c r="C49" s="44" t="s">
+        <v>67</v>
       </c>
       <c r="D49" s="32" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E49" s="24" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="F49" s="25">
-        <v>45078.0</v>
+        <v>45080.0</v>
       </c>
       <c r="G49" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H49" s="26">
-        <v>0.0</v>
+      <c r="H49" s="33">
+        <v>1.0</v>
       </c>
       <c r="J49" s="34"/>
       <c r="K49" s="5"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="15"/>
-      <c r="B50" s="60" t="s">
+      <c r="B50" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>158</v>
+      </c>
+      <c r="D50" s="60" t="s">
+        <v>159</v>
+      </c>
+      <c r="E50" s="61" t="s">
         <v>160</v>
-      </c>
-      <c r="C50" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="D50" s="32" t="s">
-        <v>162</v>
-      </c>
-      <c r="E50" s="24" t="s">
-        <v>163</v>
       </c>
       <c r="F50" s="25">
         <v>45078.0</v>
@@ -2979,34 +2982,34 @@
       <c r="G50" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H50" s="26">
-        <v>0.0</v>
+      <c r="H50" s="33">
+        <v>1.0</v>
       </c>
       <c r="J50" s="34"/>
       <c r="K50" s="5"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="15"/>
-      <c r="B51" s="61" t="s">
-        <v>164</v>
-      </c>
-      <c r="C51" s="44" t="s">
-        <v>62</v>
+      <c r="B51" s="62" t="s">
+        <v>161</v>
+      </c>
+      <c r="C51" s="38" t="s">
+        <v>162</v>
       </c>
       <c r="D51" s="32" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E51" s="24" t="s">
-        <v>104</v>
+        <v>57</v>
       </c>
       <c r="F51" s="25">
-        <v>45080.0</v>
+        <v>45078.0</v>
       </c>
       <c r="G51" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H51" s="26">
-        <v>0.0</v>
+      <c r="H51" s="33">
+        <v>1.0</v>
       </c>
       <c r="J51" s="34"/>
       <c r="K51" s="5"/>
@@ -3014,25 +3017,25 @@
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="15"/>
       <c r="B52" s="62" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="D52" s="32" t="s">
         <v>166</v>
       </c>
-      <c r="C52" s="44" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="32" t="s">
+      <c r="E52" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="E52" s="24" t="s">
-        <v>69</v>
-      </c>
       <c r="F52" s="25">
-        <v>45080.0</v>
+        <v>45078.0</v>
       </c>
       <c r="G52" s="25">
         <v>45092.0</v>
       </c>
-      <c r="H52" s="26">
-        <v>0.0</v>
+      <c r="H52" s="33">
+        <v>1.0</v>
       </c>
       <c r="J52" s="34"/>
       <c r="K52" s="5"/>
@@ -5055,9 +5058,9 @@
     <row r="1017" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="I55:I57"/>
     <mergeCell ref="I58:I62"/>
     <mergeCell ref="I46:I54"/>
-    <mergeCell ref="I55:I57"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="I12:I21"/>
@@ -6268,6 +6271,23 @@
         <v>226</v>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" s="93">
+        <v>44929.0</v>
+      </c>
+      <c r="B7" s="90">
+        <v>45096.0</v>
+      </c>
+      <c r="C7" s="91" t="s">
+        <v>220</v>
+      </c>
+      <c r="D7" s="92" t="s">
+        <v>227</v>
+      </c>
+      <c r="E7" s="92" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizacion de porcentaje del cronograma del proyecto
</commit_message>
<xml_diff>
--- a/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
+++ b/02-Desarrollo/SGI/01-Documentos/SGI-CP.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="230">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -568,13 +568,13 @@
     <t>Huarhua/AS, Durand/PB</t>
   </si>
   <si>
-    <t>Generar documentación para el usuario</t>
+    <t>Generar documentación para el usuario versión Preliminar</t>
   </si>
   <si>
     <t>Manual de usuario</t>
   </si>
   <si>
-    <t>SGI-MU.DOCX</t>
+    <t>SGI-MU1.DOCX</t>
   </si>
   <si>
     <t>Soller/PB, Balceda/PB, Huarhua/UI, Del Aguila/QA</t>
@@ -595,7 +595,7 @@
     <t>SGI-RDS2.DOCX</t>
   </si>
   <si>
-    <t>Balarezo/JP, Canecillas/A, Durand/PB, Balceda/PB</t>
+    <t>Balarezo/JP, Canecillas/A, Balceda/PB</t>
   </si>
   <si>
     <t>Reporte del Tercer Sprint</t>
@@ -610,6 +610,12 @@
     <t>S9 - S10</t>
   </si>
   <si>
+    <t>Generar documentación para el usuario versión Versión Final</t>
+  </si>
+  <si>
+    <t>SGI-MU2.DOCX</t>
+  </si>
+  <si>
     <t>Documentar Acta de finalización del Hito 3</t>
   </si>
   <si>
@@ -619,7 +625,7 @@
     <t>SGI-AFH3.DOCX</t>
   </si>
   <si>
-    <t>Balarezo/JP, Del Aguila/QA, Soller/PB</t>
+    <t>Justiniano/A, Del Aguila/QA, Soller/PB</t>
   </si>
   <si>
     <t>Elaborar del acta de cierre del proyecto</t>
@@ -3060,15 +3066,15 @@
       <c r="G53" s="25">
         <v>45097.0</v>
       </c>
-      <c r="H53" s="26">
-        <v>0.0</v>
+      <c r="H53" s="33">
+        <v>1.0</v>
       </c>
       <c r="J53" s="34"/>
       <c r="K53" s="5"/>
     </row>
     <row r="54" ht="14.25" customHeight="1">
       <c r="A54" s="15"/>
-      <c r="B54" s="63" t="s">
+      <c r="B54" s="62" t="s">
         <v>171</v>
       </c>
       <c r="C54" s="36" t="s">
@@ -3086,8 +3092,8 @@
       <c r="G54" s="25">
         <v>45097.0</v>
       </c>
-      <c r="H54" s="26">
-        <v>0.0</v>
+      <c r="H54" s="33">
+        <v>1.0</v>
       </c>
       <c r="J54" s="34"/>
       <c r="K54" s="5"/>
@@ -3112,8 +3118,8 @@
       <c r="G55" s="25">
         <v>45101.0</v>
       </c>
-      <c r="H55" s="26">
-        <v>0.0</v>
+      <c r="H55" s="33">
+        <v>1.0</v>
       </c>
       <c r="I55" s="27" t="s">
         <v>176</v>
@@ -3141,8 +3147,8 @@
       <c r="G56" s="25">
         <v>45107.0</v>
       </c>
-      <c r="H56" s="26">
-        <v>0.0</v>
+      <c r="H56" s="33">
+        <v>1.0</v>
       </c>
       <c r="J56" s="34"/>
       <c r="K56" s="5"/>
@@ -3167,8 +3173,8 @@
       <c r="G57" s="25">
         <v>45107.0</v>
       </c>
-      <c r="H57" s="26">
-        <v>0.0</v>
+      <c r="H57" s="33">
+        <v>1.0</v>
       </c>
       <c r="J57" s="34"/>
       <c r="K57" s="5"/>
@@ -3193,8 +3199,8 @@
       <c r="G58" s="25">
         <v>45107.0</v>
       </c>
-      <c r="H58" s="26">
-        <v>0.0</v>
+      <c r="H58" s="33">
+        <v>1.0</v>
       </c>
       <c r="I58" s="27" t="s">
         <v>184</v>
@@ -3204,17 +3210,17 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="15"/>
-      <c r="B59" s="37" t="s">
+      <c r="B59" s="62" t="s">
         <v>185</v>
       </c>
-      <c r="C59" s="38" t="s">
+      <c r="C59" s="36" t="s">
+        <v>172</v>
+      </c>
+      <c r="D59" s="32" t="s">
         <v>186</v>
       </c>
-      <c r="D59" s="32" t="s">
-        <v>187</v>
-      </c>
       <c r="E59" s="24" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
       <c r="F59" s="25">
         <v>45103.0</v>
@@ -3222,25 +3228,25 @@
       <c r="G59" s="25">
         <v>45107.0</v>
       </c>
-      <c r="H59" s="26">
-        <v>0.0</v>
+      <c r="H59" s="33">
+        <v>1.0</v>
       </c>
       <c r="J59" s="34"/>
       <c r="K59" s="5"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="15"/>
-      <c r="B60" s="64" t="s">
+      <c r="B60" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="C60" s="38" t="s">
+        <v>188</v>
+      </c>
+      <c r="D60" s="32" t="s">
         <v>189</v>
       </c>
-      <c r="C60" s="65" t="s">
+      <c r="E60" s="24" t="s">
         <v>190</v>
-      </c>
-      <c r="D60" s="32" t="s">
-        <v>191</v>
-      </c>
-      <c r="E60" s="24" t="s">
-        <v>192</v>
       </c>
       <c r="F60" s="25">
         <v>45103.0</v>
@@ -3248,25 +3254,25 @@
       <c r="G60" s="25">
         <v>45107.0</v>
       </c>
-      <c r="H60" s="26">
-        <v>0.0</v>
+      <c r="H60" s="33">
+        <v>1.0</v>
       </c>
       <c r="J60" s="34"/>
       <c r="K60" s="5"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="15"/>
-      <c r="B61" s="37" t="s">
+      <c r="B61" s="64" t="s">
+        <v>191</v>
+      </c>
+      <c r="C61" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="C61" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D61" s="32" t="s">
-        <v>21</v>
-      </c>
       <c r="E61" s="24" t="s">
-        <v>34</v>
+        <v>194</v>
       </c>
       <c r="F61" s="25">
         <v>45103.0</v>
@@ -3275,43 +3281,64 @@
         <v>45107.0</v>
       </c>
       <c r="H61" s="33">
-        <v>0.0</v>
-      </c>
+        <v>1.0</v>
+      </c>
+      <c r="J61" s="34"/>
+      <c r="K61" s="5"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="B62" s="66" t="s">
+      <c r="A62" s="15"/>
+      <c r="B62" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="C62" s="67"/>
-      <c r="D62" s="68"/>
-      <c r="E62" s="69"/>
-      <c r="F62" s="70">
+      <c r="C62" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="D62" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F62" s="25">
+        <v>45103.0</v>
+      </c>
+      <c r="G62" s="25">
+        <v>45107.0</v>
+      </c>
+      <c r="H62" s="33">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="63" ht="15.75" customHeight="1">
+      <c r="A63" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="B63" s="66" t="s">
+        <v>197</v>
+      </c>
+      <c r="C63" s="67"/>
+      <c r="D63" s="68"/>
+      <c r="E63" s="69"/>
+      <c r="F63" s="70">
         <v>45078.0</v>
       </c>
-      <c r="G62" s="70">
+      <c r="G63" s="70">
         <v>45107.0</v>
       </c>
-      <c r="H62" s="71"/>
-    </row>
-    <row r="63" ht="15.75" customHeight="1">
-      <c r="B63" s="72"/>
-      <c r="C63" s="72"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="72"/>
-      <c r="F63" s="73"/>
-      <c r="G63" s="73"/>
-      <c r="H63" s="73"/>
+      <c r="H63" s="71"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="B64" s="74"/>
-      <c r="F64" s="7"/>
-      <c r="G64" s="7"/>
-      <c r="H64" s="7"/>
+      <c r="B64" s="72"/>
+      <c r="C64" s="72"/>
+      <c r="D64" s="72"/>
+      <c r="E64" s="72"/>
+      <c r="F64" s="73"/>
+      <c r="G64" s="73"/>
+      <c r="H64" s="73"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
+      <c r="B65" s="74"/>
       <c r="F65" s="7"/>
       <c r="G65" s="7"/>
       <c r="H65" s="7"/>
@@ -4301,7 +4328,11 @@
       <c r="G262" s="7"/>
       <c r="H262" s="7"/>
     </row>
-    <row r="263" ht="15.75" customHeight="1"/>
+    <row r="263" ht="15.75" customHeight="1">
+      <c r="F263" s="7"/>
+      <c r="G263" s="7"/>
+      <c r="H263" s="7"/>
+    </row>
     <row r="264" ht="15.75" customHeight="1"/>
     <row r="265" ht="15.75" customHeight="1"/>
     <row r="266" ht="15.75" customHeight="1"/>
@@ -5056,11 +5087,12 @@
     <row r="1015" ht="15.75" customHeight="1"/>
     <row r="1016" ht="15.75" customHeight="1"/>
     <row r="1017" ht="15.75" customHeight="1"/>
+    <row r="1018" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="I55:I57"/>
-    <mergeCell ref="I58:I62"/>
     <mergeCell ref="I46:I54"/>
+    <mergeCell ref="I58:I63"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="I12:I21"/>
@@ -5099,86 +5131,86 @@
     <row r="1" ht="15.75" customHeight="1"/>
     <row r="2" ht="15.75" customHeight="1">
       <c r="B2" s="75" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C2" s="15"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="B3" s="76" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C3" s="4"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="B4" s="77" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="C4" s="78" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="B5" s="79" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="C5" s="80" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="B6" s="79" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="B7" s="79" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="B8" s="81" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="C8" s="80" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="B9" s="79" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="B10" s="79" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C10" s="80" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="B11" s="82" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="C11" s="83" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="B12" s="84" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C12" s="85" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1"/>
@@ -6188,33 +6220,33 @@
   <sheetData>
     <row r="2">
       <c r="A2" s="86" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="B2" s="87" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C2" s="87" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="D2" s="87" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="E2" s="88" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="89" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B3" s="90">
         <v>45024.0</v>
       </c>
       <c r="C3" s="91" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D3" s="92" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="E3" s="91" t="s">
         <v>21</v>
@@ -6228,10 +6260,10 @@
         <v>45047.0</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D4" s="92" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="E4" s="91" t="s">
         <v>21</v>
@@ -6245,10 +6277,10 @@
         <v>45047.0</v>
       </c>
       <c r="C5" s="91" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D5" s="92" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="E5" s="91" t="s">
         <v>21</v>
@@ -6256,19 +6288,19 @@
     </row>
     <row r="6">
       <c r="A6" s="94" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="B6" s="90">
         <v>45053.0</v>
       </c>
       <c r="C6" s="91" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D6" s="92" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="E6" s="92" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
     </row>
     <row r="7">
@@ -6279,14 +6311,27 @@
         <v>45096.0</v>
       </c>
       <c r="C7" s="91" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D7" s="92" t="s">
-        <v>227</v>
-      </c>
-      <c r="E7" s="92" t="s">
-        <v>226</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="E7" s="92"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="93">
+        <v>44960.0</v>
+      </c>
+      <c r="B8" s="90">
+        <v>45107.0</v>
+      </c>
+      <c r="C8" s="91" t="s">
+        <v>222</v>
+      </c>
+      <c r="D8" s="92" t="s">
+        <v>229</v>
+      </c>
+      <c r="E8" s="92"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>